<commit_message>
Resolved bug with Providers
Name was not populating due to putting in a copy and paste.
</commit_message>
<xml_diff>
--- a/working/providers/providers.xlsx
+++ b/working/providers/providers.xlsx
@@ -46,7 +46,7 @@
     <t>JANSAN</t>
   </si>
   <si>
-    <t>GS-07F-BA385</t>
+    <t>GS07FBA385</t>
   </si>
   <si>
     <t>usg</t>
@@ -73,7 +73,7 @@
     <t>JANSAN</t>
   </si>
   <si>
-    <t>GS-07F-BA386</t>
+    <t>GS07FBA386</t>
   </si>
   <si>
     <t>usg</t>
@@ -100,7 +100,7 @@
     <t>JANSAN</t>
   </si>
   <si>
-    <t>GS-07F-BA387</t>
+    <t>GS07FBA387</t>
   </si>
   <si>
     <t>usg</t>
@@ -127,7 +127,7 @@
     <t>JANSAN</t>
   </si>
   <si>
-    <t>GS-07F-BA388</t>
+    <t>GS07FBA388</t>
   </si>
   <si>
     <t>usg</t>
@@ -154,7 +154,7 @@
     <t>JANSAN</t>
   </si>
   <si>
-    <t>GS-07F-BA390</t>
+    <t>GS07FBA390</t>
   </si>
   <si>
     <t>usg</t>
@@ -181,7 +181,7 @@
     <t>JANSAN</t>
   </si>
   <si>
-    <t>GS-07F-BA391</t>
+    <t>GS07FBA391</t>
   </si>
   <si>
     <t>usg</t>
@@ -208,7 +208,7 @@
     <t>JANSAN</t>
   </si>
   <si>
-    <t>GS-07F-BA389</t>
+    <t>GS07FBA389</t>
   </si>
   <si>
     <t>usg</t>
@@ -235,7 +235,7 @@
     <t>JANSAN</t>
   </si>
   <si>
-    <t>GS-07F-BA394</t>
+    <t>GS07FBA394</t>
   </si>
   <si>
     <t>usg</t>
@@ -262,7 +262,7 @@
     <t>JANSAN</t>
   </si>
   <si>
-    <t>GS-07F-BA396</t>
+    <t>GS07FBA396</t>
   </si>
   <si>
     <t>usg</t>
@@ -289,7 +289,7 @@
     <t>JANSAN</t>
   </si>
   <si>
-    <t>GS-07F-BA400</t>
+    <t>GS07FBA400</t>
   </si>
   <si>
     <t>usg</t>
@@ -316,7 +316,7 @@
     <t>JANSAN</t>
   </si>
   <si>
-    <t>GS-07F-BA401</t>
+    <t>GS07FBA401</t>
   </si>
   <si>
     <t>usg</t>
@@ -343,7 +343,7 @@
     <t>JANSAN</t>
   </si>
   <si>
-    <t>GS-07F-BA392</t>
+    <t>GS07FBA392</t>
   </si>
   <si>
     <t>usg</t>
@@ -370,7 +370,7 @@
     <t>JANSAN</t>
   </si>
   <si>
-    <t>GS-07F-BA407</t>
+    <t>GS07FBA407</t>
   </si>
   <si>
     <t>usg</t>
@@ -397,7 +397,7 @@
     <t>JANSAN</t>
   </si>
   <si>
-    <t>GS-07F-BA393</t>
+    <t>GS07FBA393</t>
   </si>
   <si>
     <t>usg</t>
@@ -424,7 +424,7 @@
     <t>JANSAN</t>
   </si>
   <si>
-    <t>GS-07F-BA395</t>
+    <t>GS07FBA395</t>
   </si>
   <si>
     <t>usg</t>
@@ -451,7 +451,7 @@
     <t>JANSAN</t>
   </si>
   <si>
-    <t>GS-07F-BA397</t>
+    <t>GS07FBA397</t>
   </si>
   <si>
     <t>usg</t>
@@ -478,7 +478,7 @@
     <t>JANSAN</t>
   </si>
   <si>
-    <t>GS-07F-BA398</t>
+    <t>GS07FBA398</t>
   </si>
   <si>
     <t>usg</t>
@@ -505,7 +505,7 @@
     <t>JANSAN</t>
   </si>
   <si>
-    <t>GS-07F-BA399</t>
+    <t>GS07FBA399</t>
   </si>
   <si>
     <t>usg</t>
@@ -532,7 +532,7 @@
     <t>PM</t>
   </si>
   <si>
-    <t>GS-03F-AA005</t>
+    <t>GS03FAA005</t>
   </si>
   <si>
     <t>usg</t>
@@ -559,7 +559,7 @@
     <t>PM</t>
   </si>
   <si>
-    <t>GS-03F-AA004</t>
+    <t>GS03FAA004</t>
   </si>
   <si>
     <t>usg</t>
@@ -586,7 +586,7 @@
     <t>PM</t>
   </si>
   <si>
-    <t>GS-03F-AA006</t>
+    <t>GS03FAA006</t>
   </si>
   <si>
     <t>usg</t>
@@ -613,7 +613,7 @@
     <t>PM</t>
   </si>
   <si>
-    <t>GS-03F-PM003</t>
+    <t>GS03FPM003</t>
   </si>
   <si>
     <t>usg</t>
@@ -640,7 +640,7 @@
     <t>PM</t>
   </si>
   <si>
-    <t>GS-03F-PM004</t>
+    <t>GS03FPM004</t>
   </si>
   <si>
     <t>usg</t>
@@ -667,7 +667,7 @@
     <t>PM</t>
   </si>
   <si>
-    <t>GS-03F-PM005</t>
+    <t>GS03FPM005</t>
   </si>
   <si>
     <t>usg</t>
@@ -694,7 +694,7 @@
     <t>PM</t>
   </si>
   <si>
-    <t>GS-03F-PM009</t>
+    <t>GS03FPM009</t>
   </si>
   <si>
     <t>usg</t>
@@ -721,7 +721,7 @@
     <t>PM</t>
   </si>
   <si>
-    <t>GS-03F-PM008</t>
+    <t>GS03FPM008</t>
   </si>
   <si>
     <t>usg</t>
@@ -748,7 +748,7 @@
     <t>PM</t>
   </si>
   <si>
-    <t>GS-03F-PM010</t>
+    <t>GS03FPM010</t>
   </si>
   <si>
     <t>usg</t>
@@ -775,7 +775,7 @@
     <t>PM</t>
   </si>
   <si>
-    <t>GS-03F-PM001</t>
+    <t>GS03FPM001</t>
   </si>
   <si>
     <t>usg</t>
@@ -802,7 +802,7 @@
     <t>PM</t>
   </si>
   <si>
-    <t>GS-03F-PM006</t>
+    <t>GS03FPM006</t>
   </si>
   <si>
     <t>usg</t>
@@ -829,7 +829,7 @@
     <t>PM</t>
   </si>
   <si>
-    <t>GS-03F-PM007</t>
+    <t>GS03FPM007</t>
   </si>
   <si>
     <t>usg</t>
@@ -856,7 +856,7 @@
     <t>PM</t>
   </si>
   <si>
-    <t>GS-03F-PM011</t>
+    <t>GS03FPM011</t>
   </si>
   <si>
     <t>usg</t>
@@ -991,7 +991,7 @@
     <t>MRO</t>
   </si>
   <si>
-    <t>GS-23F-BA005</t>
+    <t>GS23FBA005</t>
   </si>
   <si>
     <t>usg</t>
@@ -1018,7 +1018,7 @@
     <t>MRO</t>
   </si>
   <si>
-    <t>GS-23F-BA017</t>
+    <t>GS23FBA017</t>
   </si>
   <si>
     <t>usg</t>
@@ -1045,7 +1045,7 @@
     <t>MRO</t>
   </si>
   <si>
-    <t>GS-23F-BA016</t>
+    <t>GS23FBA016</t>
   </si>
   <si>
     <t>usg</t>
@@ -1072,7 +1072,7 @@
     <t>MRO</t>
   </si>
   <si>
-    <t>GS-23F-BA006</t>
+    <t>GS23FBA006</t>
   </si>
   <si>
     <t>usg</t>
@@ -1099,7 +1099,7 @@
     <t>MRO</t>
   </si>
   <si>
-    <t>GS-23F-BA007</t>
+    <t>GS23FBA007</t>
   </si>
   <si>
     <t>usg</t>
@@ -1126,7 +1126,7 @@
     <t>MRO</t>
   </si>
   <si>
-    <t>GS-23F-BA008</t>
+    <t>GS23FBA008</t>
   </si>
   <si>
     <t>usg</t>
@@ -1153,7 +1153,7 @@
     <t>MRO</t>
   </si>
   <si>
-    <t>GS-23F-BA009</t>
+    <t>GS23FBA009</t>
   </si>
   <si>
     <t>usg</t>
@@ -1180,7 +1180,7 @@
     <t>MRO</t>
   </si>
   <si>
-    <t>GS-23F-BA012</t>
+    <t>GS23FBA012</t>
   </si>
   <si>
     <t>usg</t>
@@ -1207,7 +1207,7 @@
     <t>MRO</t>
   </si>
   <si>
-    <t>GS-23F-BA013</t>
+    <t>GS23FBA013</t>
   </si>
   <si>
     <t>usg</t>
@@ -1234,7 +1234,7 @@
     <t>MRO</t>
   </si>
   <si>
-    <t>GS-23F-BA014</t>
+    <t>GS23FBA014</t>
   </si>
   <si>
     <t>usg</t>
@@ -1261,7 +1261,7 @@
     <t>MRO</t>
   </si>
   <si>
-    <t>GS-23F-BA015</t>
+    <t>GS23FBA015</t>
   </si>
   <si>
     <t>usg</t>
@@ -1288,7 +1288,7 @@
     <t>DDS3</t>
   </si>
   <si>
-    <t>GS-33F-BA016</t>
+    <t>GS33FBA016</t>
   </si>
   <si>
     <t>usg</t>
@@ -1315,7 +1315,7 @@
     <t>DDS3</t>
   </si>
   <si>
-    <t>GS-33F-CA001</t>
+    <t>GS33FCA001</t>
   </si>
   <si>
     <t>usg</t>
@@ -1674,8 +1674,9 @@
     <col min="4" customWidth="1" max="4" width="17.29"/>
     <col min="5" customWidth="1" max="5" width="19.43"/>
     <col min="6" customWidth="1" max="6" width="23.0"/>
-    <col min="7" customWidth="1" max="8" width="26.29"/>
-    <col min="9" customWidth="1" max="9" width="18.71"/>
+    <col min="7" customWidth="1" max="7" width="26.29"/>
+    <col min="8" customWidth="1" max="8" width="29.29"/>
+    <col min="9" customWidth="1" max="9" width="25.29"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1714,7 +1715,7 @@
       <c t="s" s="1" r="B2">
         <v>10</v>
       </c>
-      <c t="s" s="1" r="C2">
+      <c t="s" s="2" r="C2">
         <v>11</v>
       </c>
       <c t="s" s="2" r="D2">
@@ -1743,7 +1744,7 @@
       <c t="s" s="1" r="B3">
         <v>19</v>
       </c>
-      <c t="s" s="1" r="C3">
+      <c t="s" s="2" r="C3">
         <v>20</v>
       </c>
       <c t="s" s="2" r="D3">
@@ -1772,7 +1773,7 @@
       <c t="s" s="1" r="B4">
         <v>28</v>
       </c>
-      <c t="s" s="1" r="C4">
+      <c t="s" s="2" r="C4">
         <v>29</v>
       </c>
       <c t="s" s="2" r="D4">
@@ -1801,7 +1802,7 @@
       <c t="s" s="1" r="B5">
         <v>37</v>
       </c>
-      <c t="s" s="1" r="C5">
+      <c t="s" s="2" r="C5">
         <v>38</v>
       </c>
       <c t="s" s="2" r="D5">
@@ -1830,7 +1831,7 @@
       <c t="s" s="1" r="B6">
         <v>46</v>
       </c>
-      <c t="s" s="1" r="C6">
+      <c t="s" s="2" r="C6">
         <v>47</v>
       </c>
       <c t="s" s="2" r="D6">
@@ -1859,7 +1860,7 @@
       <c t="s" s="1" r="B7">
         <v>55</v>
       </c>
-      <c t="s" s="1" r="C7">
+      <c t="s" s="2" r="C7">
         <v>56</v>
       </c>
       <c t="s" s="2" r="D7">
@@ -1888,7 +1889,7 @@
       <c t="s" s="1" r="B8">
         <v>64</v>
       </c>
-      <c t="s" s="1" r="C8">
+      <c t="s" s="2" r="C8">
         <v>65</v>
       </c>
       <c t="s" s="2" r="D8">
@@ -1917,7 +1918,7 @@
       <c t="s" s="1" r="B9">
         <v>73</v>
       </c>
-      <c t="s" s="1" r="C9">
+      <c t="s" s="2" r="C9">
         <v>74</v>
       </c>
       <c t="s" s="2" r="D9">
@@ -1946,7 +1947,7 @@
       <c t="s" s="1" r="B10">
         <v>82</v>
       </c>
-      <c t="s" s="1" r="C10">
+      <c t="s" s="2" r="C10">
         <v>83</v>
       </c>
       <c t="s" s="2" r="D10">
@@ -1975,7 +1976,7 @@
       <c t="s" s="1" r="B11">
         <v>91</v>
       </c>
-      <c t="s" s="1" r="C11">
+      <c t="s" s="2" r="C11">
         <v>92</v>
       </c>
       <c t="s" s="2" r="D11">
@@ -2004,7 +2005,7 @@
       <c t="s" s="1" r="B12">
         <v>100</v>
       </c>
-      <c t="s" s="1" r="C12">
+      <c t="s" s="2" r="C12">
         <v>101</v>
       </c>
       <c t="s" s="2" r="D12">
@@ -2033,7 +2034,7 @@
       <c t="s" s="1" r="B13">
         <v>109</v>
       </c>
-      <c t="s" s="1" r="C13">
+      <c t="s" s="2" r="C13">
         <v>110</v>
       </c>
       <c t="s" s="2" r="D13">
@@ -2062,7 +2063,7 @@
       <c t="s" s="1" r="B14">
         <v>118</v>
       </c>
-      <c t="s" s="1" r="C14">
+      <c t="s" s="2" r="C14">
         <v>119</v>
       </c>
       <c t="s" s="2" r="D14">
@@ -2091,7 +2092,7 @@
       <c t="s" s="1" r="B15">
         <v>127</v>
       </c>
-      <c t="s" s="1" r="C15">
+      <c t="s" s="2" r="C15">
         <v>128</v>
       </c>
       <c t="s" s="2" r="D15">
@@ -2120,7 +2121,7 @@
       <c t="s" s="1" r="B16">
         <v>136</v>
       </c>
-      <c t="s" s="1" r="C16">
+      <c t="s" s="2" r="C16">
         <v>137</v>
       </c>
       <c t="s" s="2" r="D16">
@@ -2149,7 +2150,7 @@
       <c t="s" s="1" r="B17">
         <v>145</v>
       </c>
-      <c t="s" s="1" r="C17">
+      <c t="s" s="2" r="C17">
         <v>146</v>
       </c>
       <c t="s" s="2" r="D17">
@@ -2178,7 +2179,7 @@
       <c t="s" s="1" r="B18">
         <v>154</v>
       </c>
-      <c t="s" s="1" r="C18">
+      <c t="s" s="2" r="C18">
         <v>155</v>
       </c>
       <c t="s" s="2" r="D18">
@@ -2207,7 +2208,7 @@
       <c t="s" s="1" r="B19">
         <v>163</v>
       </c>
-      <c t="s" s="1" r="C19">
+      <c t="s" s="2" r="C19">
         <v>164</v>
       </c>
       <c t="s" s="2" r="D19">
@@ -2236,7 +2237,7 @@
       <c t="s" s="1" r="B20">
         <v>172</v>
       </c>
-      <c t="s" s="1" r="C20">
+      <c t="s" s="2" r="C20">
         <v>173</v>
       </c>
       <c t="s" s="2" r="D20">
@@ -2265,7 +2266,7 @@
       <c t="s" s="1" r="B21">
         <v>181</v>
       </c>
-      <c t="s" s="1" r="C21">
+      <c t="s" s="2" r="C21">
         <v>182</v>
       </c>
       <c t="s" s="2" r="D21">
@@ -2294,7 +2295,7 @@
       <c t="s" s="1" r="B22">
         <v>190</v>
       </c>
-      <c t="s" s="1" r="C22">
+      <c t="s" s="2" r="C22">
         <v>191</v>
       </c>
       <c t="s" s="2" r="D22">
@@ -2323,7 +2324,7 @@
       <c t="s" s="1" r="B23">
         <v>199</v>
       </c>
-      <c t="s" s="1" r="C23">
+      <c t="s" s="2" r="C23">
         <v>200</v>
       </c>
       <c t="s" s="2" r="D23">
@@ -2352,7 +2353,7 @@
       <c t="s" s="1" r="B24">
         <v>208</v>
       </c>
-      <c t="s" s="1" r="C24">
+      <c t="s" s="2" r="C24">
         <v>209</v>
       </c>
       <c t="s" s="2" r="D24">
@@ -2381,7 +2382,7 @@
       <c t="s" s="1" r="B25">
         <v>217</v>
       </c>
-      <c t="s" s="1" r="C25">
+      <c t="s" s="2" r="C25">
         <v>218</v>
       </c>
       <c t="s" s="2" r="D25">
@@ -2410,7 +2411,7 @@
       <c t="s" s="1" r="B26">
         <v>226</v>
       </c>
-      <c t="s" s="1" r="C26">
+      <c t="s" s="2" r="C26">
         <v>227</v>
       </c>
       <c t="s" s="2" r="D26">
@@ -2439,7 +2440,7 @@
       <c t="s" s="1" r="B27">
         <v>235</v>
       </c>
-      <c t="s" s="1" r="C27">
+      <c t="s" s="2" r="C27">
         <v>236</v>
       </c>
       <c t="s" s="2" r="D27">
@@ -2468,7 +2469,7 @@
       <c t="s" s="1" r="B28">
         <v>244</v>
       </c>
-      <c t="s" s="1" r="C28">
+      <c t="s" s="2" r="C28">
         <v>245</v>
       </c>
       <c t="s" s="2" r="D28">
@@ -2497,7 +2498,7 @@
       <c t="s" s="1" r="B29">
         <v>253</v>
       </c>
-      <c t="s" s="1" r="C29">
+      <c t="s" s="2" r="C29">
         <v>254</v>
       </c>
       <c t="s" s="2" r="D29">
@@ -2526,7 +2527,7 @@
       <c t="s" s="1" r="B30">
         <v>262</v>
       </c>
-      <c t="s" s="1" r="C30">
+      <c t="s" s="2" r="C30">
         <v>263</v>
       </c>
       <c t="s" s="2" r="D30">
@@ -2555,7 +2556,7 @@
       <c t="s" s="1" r="B31">
         <v>271</v>
       </c>
-      <c t="s" s="1" r="C31">
+      <c t="s" s="2" r="C31">
         <v>272</v>
       </c>
       <c t="s" s="2" r="D31">
@@ -2584,7 +2585,7 @@
       <c t="s" s="1" r="B32">
         <v>280</v>
       </c>
-      <c t="s" s="1" r="C32">
+      <c t="s" s="2" r="C32">
         <v>281</v>
       </c>
       <c t="s" s="2" r="D32">
@@ -2729,7 +2730,7 @@
       <c t="s" s="1" r="B37">
         <v>325</v>
       </c>
-      <c t="s" s="1" r="C37">
+      <c t="s" s="2" r="C37">
         <v>326</v>
       </c>
       <c t="s" s="2" r="D37">
@@ -2758,7 +2759,7 @@
       <c t="s" s="1" r="B38">
         <v>334</v>
       </c>
-      <c t="s" s="1" r="C38">
+      <c t="s" s="2" r="C38">
         <v>335</v>
       </c>
       <c t="s" s="2" r="D38">
@@ -2787,7 +2788,7 @@
       <c t="s" s="1" r="B39">
         <v>343</v>
       </c>
-      <c t="s" s="1" r="C39">
+      <c t="s" s="2" r="C39">
         <v>344</v>
       </c>
       <c t="s" s="2" r="D39">
@@ -2816,7 +2817,7 @@
       <c t="s" s="1" r="B40">
         <v>352</v>
       </c>
-      <c t="s" s="1" r="C40">
+      <c t="s" s="2" r="C40">
         <v>353</v>
       </c>
       <c t="s" s="2" r="D40">
@@ -2845,7 +2846,7 @@
       <c t="s" s="1" r="B41">
         <v>361</v>
       </c>
-      <c t="s" s="1" r="C41">
+      <c t="s" s="2" r="C41">
         <v>362</v>
       </c>
       <c t="s" s="2" r="D41">
@@ -2874,7 +2875,7 @@
       <c t="s" s="1" r="B42">
         <v>370</v>
       </c>
-      <c t="s" s="1" r="C42">
+      <c t="s" s="2" r="C42">
         <v>371</v>
       </c>
       <c t="s" s="2" r="D42">
@@ -2903,7 +2904,7 @@
       <c t="s" s="1" r="B43">
         <v>379</v>
       </c>
-      <c t="s" s="1" r="C43">
+      <c t="s" s="2" r="C43">
         <v>380</v>
       </c>
       <c t="s" s="2" r="D43">
@@ -2932,7 +2933,7 @@
       <c t="s" s="1" r="B44">
         <v>388</v>
       </c>
-      <c t="s" s="1" r="C44">
+      <c t="s" s="2" r="C44">
         <v>389</v>
       </c>
       <c t="s" s="2" r="D44">
@@ -2961,7 +2962,7 @@
       <c t="s" s="1" r="B45">
         <v>397</v>
       </c>
-      <c t="s" s="1" r="C45">
+      <c t="s" s="2" r="C45">
         <v>398</v>
       </c>
       <c t="s" s="2" r="D45">
@@ -2990,7 +2991,7 @@
       <c t="s" s="1" r="B46">
         <v>406</v>
       </c>
-      <c t="s" s="1" r="C46">
+      <c t="s" s="2" r="C46">
         <v>407</v>
       </c>
       <c t="s" s="2" r="D46">
@@ -3019,7 +3020,7 @@
       <c t="s" s="1" r="B47">
         <v>415</v>
       </c>
-      <c t="s" s="1" r="C47">
+      <c t="s" s="2" r="C47">
         <v>416</v>
       </c>
       <c t="s" s="2" r="D47">
@@ -3048,7 +3049,7 @@
       <c t="s" s="1" r="B48">
         <v>424</v>
       </c>
-      <c t="s" s="1" r="C48">
+      <c t="s" s="2" r="C48">
         <v>425</v>
       </c>
       <c t="s" s="2" r="D48">
@@ -3077,7 +3078,7 @@
       <c t="s" s="1" r="B49">
         <v>433</v>
       </c>
-      <c t="s" s="1" r="C49">
+      <c t="s" s="2" r="C49">
         <v>434</v>
       </c>
       <c t="s" s="2" r="D49">

</xml_diff>

<commit_message>
Schemas now push effectivedates down to the constraint level. Also included a lot of error checking with the Schema's XML ingest
</commit_message>
<xml_diff>
--- a/working/providers/providers.xlsx
+++ b/working/providers/providers.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="1515" yWindow="585" windowWidth="15780" windowHeight="6855"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="239">
   <si>
     <t>PROVIDER_ID</t>
   </si>
@@ -40,9 +43,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -55,9 +55,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -70,9 +67,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -85,9 +79,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -100,9 +91,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -115,9 +103,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -130,9 +115,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -145,9 +127,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -160,9 +139,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -175,9 +151,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -190,9 +163,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -205,9 +175,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -220,9 +187,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -235,9 +199,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -250,9 +211,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -265,9 +223,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -280,9 +235,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -295,9 +247,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>004</t>
   </si>
   <si>
@@ -310,9 +259,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>004</t>
   </si>
   <si>
@@ -325,9 +271,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>004</t>
   </si>
   <si>
@@ -340,9 +283,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>004</t>
   </si>
   <si>
@@ -355,9 +295,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>004</t>
   </si>
   <si>
@@ -370,9 +307,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>004</t>
   </si>
   <si>
@@ -385,9 +319,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>004</t>
   </si>
   <si>
@@ -400,9 +331,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>004</t>
   </si>
   <si>
@@ -415,9 +343,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>004</t>
   </si>
   <si>
@@ -430,9 +355,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>004</t>
   </si>
   <si>
@@ -445,9 +367,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>004</t>
   </si>
   <si>
@@ -460,9 +379,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>004</t>
   </si>
   <si>
@@ -475,9 +391,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>004</t>
   </si>
   <si>
@@ -490,9 +403,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>005</t>
   </si>
   <si>
@@ -505,9 +415,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>005</t>
   </si>
   <si>
@@ -520,9 +427,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>005</t>
   </si>
   <si>
@@ -535,9 +439,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>005</t>
   </si>
   <si>
@@ -550,9 +451,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -565,9 +463,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -580,9 +475,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -595,9 +487,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -610,9 +499,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -625,9 +511,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -640,9 +523,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -655,9 +535,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -670,9 +547,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -685,9 +559,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -700,9 +571,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -715,9 +583,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>006</t>
   </si>
   <si>
@@ -730,9 +595,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>006</t>
   </si>
   <si>
@@ -745,9 +607,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>003</t>
   </si>
   <si>
@@ -760,9 +619,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>003</t>
   </si>
   <si>
@@ -775,9 +631,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>003</t>
   </si>
   <si>
@@ -790,9 +643,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>003</t>
   </si>
   <si>
@@ -805,9 +655,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>003</t>
   </si>
   <si>
@@ -820,9 +667,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>003</t>
   </si>
   <si>
@@ -835,9 +679,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>003</t>
   </si>
   <si>
@@ -850,9 +691,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>003</t>
   </si>
   <si>
@@ -865,9 +703,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>003</t>
   </si>
   <si>
@@ -880,9 +715,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>003</t>
   </si>
   <si>
@@ -895,26 +727,32 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
+    <t>xlsx</t>
+  </si>
+  <si>
+    <t>xls</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
@@ -930,1047 +768,1336 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
-    <xf fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1"/>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
-      <alignment/>
-    </xf>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" customWidth="1" max="2" width="22.29"/>
-    <col min="3" customWidth="1" max="3" width="26.43"/>
-    <col min="4" customWidth="1" max="4" width="26.29"/>
-    <col min="5" customWidth="1" max="5" width="23.0"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c t="s" s="1" r="A1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c t="s" s="1" r="B1">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c t="s" s="1" r="C1">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="2" r="D1">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c t="s" s="2" r="E1">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c t="s" s="2" r="A2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c t="s" s="1" r="B2">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c t="s" s="2" r="C2">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="2" r="D2">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c t="s" s="2" r="E2">
+      <c r="E2" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3">
-      <c t="s" s="2" r="A3">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c t="s" s="1" r="B3">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c t="s" s="2" r="C3">
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c t="s" s="2" r="D3">
+      <c r="E3" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c t="s" s="2" r="E3">
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4">
-      <c t="s" s="2" r="A4">
+      <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
-      <c t="s" s="1" r="B4">
+      <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c t="s" s="2" r="C4">
+      <c r="E4" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
-      <c t="s" s="2" r="D4">
+      <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c t="s" s="2" r="E4">
+      <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5">
-      <c t="s" s="2" r="A5">
+      <c r="D5" s="2" t="s">
         <v>20</v>
       </c>
-      <c t="s" s="1" r="B5">
+      <c r="E5" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
-      <c t="s" s="2" r="C5">
+      <c r="B6" s="1" t="s">
         <v>22</v>
       </c>
-      <c t="s" s="2" r="D5">
+      <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
-      <c t="s" s="2" r="E5">
+      <c r="D6" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6">
-      <c t="s" s="2" r="A6">
+      <c r="E6" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c t="s" s="1" r="B6">
+      <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
-      <c t="s" s="2" r="C6">
+      <c r="C7" s="2" t="s">
         <v>27</v>
       </c>
-      <c t="s" s="2" r="D6">
+      <c r="D7" s="2" t="s">
         <v>28</v>
       </c>
-      <c t="s" s="2" r="E6">
+      <c r="E7" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7">
-      <c t="s" s="2" r="A7">
+      <c r="B8" s="1" t="s">
         <v>30</v>
       </c>
-      <c t="s" s="1" r="B7">
+      <c r="C8" s="2" t="s">
         <v>31</v>
       </c>
-      <c t="s" s="2" r="C7">
+      <c r="D8" s="2" t="s">
         <v>32</v>
       </c>
-      <c t="s" s="2" r="D7">
+      <c r="E8" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>33</v>
       </c>
-      <c t="s" s="2" r="E7">
+      <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8">
-      <c t="s" s="2" r="A8">
+      <c r="C9" s="2" t="s">
         <v>35</v>
       </c>
-      <c t="s" s="1" r="B8">
+      <c r="D9" s="2" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="2" r="C8">
+      <c r="E9" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
-      <c t="s" s="2" r="D8">
+      <c r="B10" s="1" t="s">
         <v>38</v>
       </c>
-      <c t="s" s="2" r="E8">
+      <c r="C10" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="9">
-      <c t="s" s="2" r="A9">
+      <c r="D10" s="2" t="s">
         <v>40</v>
       </c>
-      <c t="s" s="1" r="B9">
+      <c r="E10" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>41</v>
       </c>
-      <c t="s" s="2" r="C9">
+      <c r="B11" s="1" t="s">
         <v>42</v>
       </c>
-      <c t="s" s="2" r="D9">
+      <c r="C11" s="2" t="s">
         <v>43</v>
       </c>
-      <c t="s" s="2" r="E9">
+      <c r="D11" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="10">
-      <c t="s" s="2" r="A10">
+      <c r="E11" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>45</v>
       </c>
-      <c t="s" s="1" r="B10">
+      <c r="B12" s="1" t="s">
         <v>46</v>
       </c>
-      <c t="s" s="2" r="C10">
+      <c r="C12" s="2" t="s">
         <v>47</v>
       </c>
-      <c t="s" s="2" r="D10">
+      <c r="D12" s="2" t="s">
         <v>48</v>
       </c>
-      <c t="s" s="2" r="E10">
+      <c r="E12" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="11">
-      <c t="s" s="2" r="A11">
+      <c r="B13" s="1" t="s">
         <v>50</v>
       </c>
-      <c t="s" s="1" r="B11">
+      <c r="C13" s="2" t="s">
         <v>51</v>
       </c>
-      <c t="s" s="2" r="C11">
+      <c r="D13" s="2" t="s">
         <v>52</v>
       </c>
-      <c t="s" s="2" r="D11">
+      <c r="E13" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>53</v>
       </c>
-      <c t="s" s="2" r="E11">
+      <c r="B14" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="12">
-      <c t="s" s="2" r="A12">
+      <c r="C14" s="2" t="s">
         <v>55</v>
       </c>
-      <c t="s" s="1" r="B12">
+      <c r="D14" s="2" t="s">
         <v>56</v>
       </c>
-      <c t="s" s="2" r="C12">
+      <c r="E14" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>57</v>
       </c>
-      <c t="s" s="2" r="D12">
+      <c r="B15" s="1" t="s">
         <v>58</v>
       </c>
-      <c t="s" s="2" r="E12">
+      <c r="C15" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="13">
-      <c t="s" s="2" r="A13">
+      <c r="D15" s="2" t="s">
         <v>60</v>
       </c>
-      <c t="s" s="1" r="B13">
+      <c r="E15" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>61</v>
       </c>
-      <c t="s" s="2" r="C13">
+      <c r="B16" s="1" t="s">
         <v>62</v>
       </c>
-      <c t="s" s="2" r="D13">
+      <c r="C16" s="2" t="s">
         <v>63</v>
       </c>
-      <c t="s" s="2" r="E13">
+      <c r="D16" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="14">
-      <c t="s" s="2" r="A14">
+      <c r="E16" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>65</v>
       </c>
-      <c t="s" s="1" r="B14">
+      <c r="B17" s="1" t="s">
         <v>66</v>
       </c>
-      <c t="s" s="2" r="C14">
+      <c r="C17" s="2" t="s">
         <v>67</v>
       </c>
-      <c t="s" s="2" r="D14">
+      <c r="D17" s="2" t="s">
         <v>68</v>
       </c>
-      <c t="s" s="2" r="E14">
+      <c r="E17" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="15">
-      <c t="s" s="2" r="A15">
+      <c r="B18" s="1" t="s">
         <v>70</v>
       </c>
-      <c t="s" s="1" r="B15">
+      <c r="C18" s="2" t="s">
         <v>71</v>
       </c>
-      <c t="s" s="2" r="C15">
+      <c r="D18" s="2" t="s">
         <v>72</v>
       </c>
-      <c t="s" s="2" r="D15">
+      <c r="E18" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>73</v>
       </c>
-      <c t="s" s="2" r="E15">
+      <c r="B19" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="16">
-      <c t="s" s="2" r="A16">
+      <c r="C19" s="2" t="s">
         <v>75</v>
       </c>
-      <c t="s" s="1" r="B16">
+      <c r="D19" s="2" t="s">
         <v>76</v>
       </c>
-      <c t="s" s="2" r="C16">
+      <c r="E19" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>77</v>
       </c>
-      <c t="s" s="2" r="D16">
+      <c r="B20" s="1" t="s">
         <v>78</v>
       </c>
-      <c t="s" s="2" r="E16">
+      <c r="C20" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="17">
-      <c t="s" s="2" r="A17">
+      <c r="D20" s="2" t="s">
         <v>80</v>
       </c>
-      <c t="s" s="1" r="B17">
+      <c r="E20" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>81</v>
       </c>
-      <c t="s" s="2" r="C17">
+      <c r="B21" s="1" t="s">
         <v>82</v>
       </c>
-      <c t="s" s="2" r="D17">
+      <c r="C21" s="2" t="s">
         <v>83</v>
       </c>
-      <c t="s" s="2" r="E17">
+      <c r="D21" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="18">
-      <c t="s" s="2" r="A18">
+      <c r="E21" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>85</v>
       </c>
-      <c t="s" s="1" r="B18">
+      <c r="B22" s="1" t="s">
         <v>86</v>
       </c>
-      <c t="s" s="2" r="C18">
+      <c r="C22" s="2" t="s">
         <v>87</v>
       </c>
-      <c t="s" s="2" r="D18">
+      <c r="D22" s="2" t="s">
         <v>88</v>
       </c>
-      <c t="s" s="2" r="E18">
+      <c r="E22" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="19">
-      <c t="s" s="2" r="A19">
+      <c r="B23" s="1" t="s">
         <v>90</v>
       </c>
-      <c t="s" s="1" r="B19">
+      <c r="C23" s="2" t="s">
         <v>91</v>
       </c>
-      <c t="s" s="2" r="C19">
+      <c r="D23" s="2" t="s">
         <v>92</v>
       </c>
-      <c t="s" s="2" r="D19">
+      <c r="E23" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>93</v>
       </c>
-      <c t="s" s="2" r="E19">
+      <c r="B24" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="20">
-      <c t="s" s="2" r="A20">
+      <c r="C24" s="2" t="s">
         <v>95</v>
       </c>
-      <c t="s" s="1" r="B20">
+      <c r="D24" s="2" t="s">
         <v>96</v>
       </c>
-      <c t="s" s="2" r="C20">
+      <c r="E24" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>97</v>
       </c>
-      <c t="s" s="2" r="D20">
+      <c r="B25" s="1" t="s">
         <v>98</v>
       </c>
-      <c t="s" s="2" r="E20">
+      <c r="C25" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="21">
-      <c t="s" s="2" r="A21">
+      <c r="D25" s="2" t="s">
         <v>100</v>
       </c>
-      <c t="s" s="1" r="B21">
+      <c r="E25" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>101</v>
       </c>
-      <c t="s" s="2" r="C21">
+      <c r="B26" s="1" t="s">
         <v>102</v>
       </c>
-      <c t="s" s="2" r="D21">
+      <c r="C26" s="2" t="s">
         <v>103</v>
       </c>
-      <c t="s" s="2" r="E21">
+      <c r="D26" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="22">
-      <c t="s" s="2" r="A22">
+      <c r="E26" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>105</v>
       </c>
-      <c t="s" s="1" r="B22">
+      <c r="B27" s="1" t="s">
         <v>106</v>
       </c>
-      <c t="s" s="2" r="C22">
+      <c r="C27" s="2" t="s">
         <v>107</v>
       </c>
-      <c t="s" s="2" r="D22">
+      <c r="D27" s="2" t="s">
         <v>108</v>
       </c>
-      <c t="s" s="2" r="E22">
+      <c r="E27" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="23">
-      <c t="s" s="2" r="A23">
+      <c r="B28" s="1" t="s">
         <v>110</v>
       </c>
-      <c t="s" s="1" r="B23">
+      <c r="C28" s="2" t="s">
         <v>111</v>
       </c>
-      <c t="s" s="2" r="C23">
+      <c r="D28" s="2" t="s">
         <v>112</v>
       </c>
-      <c t="s" s="2" r="D23">
+      <c r="E28" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>113</v>
       </c>
-      <c t="s" s="2" r="E23">
+      <c r="B29" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="24">
-      <c t="s" s="2" r="A24">
+      <c r="C29" s="2" t="s">
         <v>115</v>
       </c>
-      <c t="s" s="1" r="B24">
+      <c r="D29" s="2" t="s">
         <v>116</v>
       </c>
-      <c t="s" s="2" r="C24">
+      <c r="E29" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>117</v>
       </c>
-      <c t="s" s="2" r="D24">
+      <c r="B30" s="1" t="s">
         <v>118</v>
       </c>
-      <c t="s" s="2" r="E24">
+      <c r="C30" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="25">
-      <c t="s" s="2" r="A25">
+      <c r="D30" s="2" t="s">
         <v>120</v>
       </c>
-      <c t="s" s="1" r="B25">
+      <c r="E30" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>121</v>
       </c>
-      <c t="s" s="2" r="C25">
+      <c r="B31" s="1" t="s">
         <v>122</v>
       </c>
-      <c t="s" s="2" r="D25">
+      <c r="C31" s="2" t="s">
         <v>123</v>
       </c>
-      <c t="s" s="2" r="E25">
+      <c r="D31" s="2" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="26">
-      <c t="s" s="2" r="A26">
+      <c r="E31" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>125</v>
       </c>
-      <c t="s" s="1" r="B26">
+      <c r="B32" s="1" t="s">
         <v>126</v>
       </c>
-      <c t="s" s="2" r="C26">
+      <c r="C32" s="2" t="s">
         <v>127</v>
       </c>
-      <c t="s" s="2" r="D26">
+      <c r="D32" s="2" t="s">
         <v>128</v>
       </c>
-      <c t="s" s="2" r="E26">
+      <c r="E32" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="27">
-      <c t="s" s="2" r="A27">
+      <c r="B33" s="1" t="s">
         <v>130</v>
       </c>
-      <c t="s" s="1" r="B27">
+      <c r="C33" s="1" t="s">
         <v>131</v>
       </c>
-      <c t="s" s="2" r="C27">
+      <c r="D33" s="2" t="s">
         <v>132</v>
       </c>
-      <c t="s" s="2" r="D27">
+      <c r="E33" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
         <v>133</v>
       </c>
-      <c t="s" s="2" r="E27">
+      <c r="B34" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="28">
-      <c t="s" s="2" r="A28">
+      <c r="C34" s="1" t="s">
         <v>135</v>
       </c>
-      <c t="s" s="1" r="B28">
+      <c r="D34" s="2" t="s">
         <v>136</v>
       </c>
-      <c t="s" s="2" r="C28">
+      <c r="E34" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>137</v>
       </c>
-      <c t="s" s="2" r="D28">
+      <c r="B35" s="1" t="s">
         <v>138</v>
       </c>
-      <c t="s" s="2" r="E28">
+      <c r="C35" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="29">
-      <c t="s" s="2" r="A29">
+      <c r="D35" s="2" t="s">
         <v>140</v>
       </c>
-      <c t="s" s="1" r="B29">
+      <c r="E35" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>141</v>
       </c>
-      <c t="s" s="2" r="C29">
+      <c r="B36" s="1" t="s">
         <v>142</v>
       </c>
-      <c t="s" s="2" r="D29">
+      <c r="C36" s="1" t="s">
         <v>143</v>
       </c>
-      <c t="s" s="2" r="E29">
+      <c r="D36" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="30">
-      <c t="s" s="2" r="A30">
+      <c r="E36" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>145</v>
       </c>
-      <c t="s" s="1" r="B30">
+      <c r="B37" s="1" t="s">
         <v>146</v>
       </c>
-      <c t="s" s="2" r="C30">
+      <c r="C37" s="2" t="s">
         <v>147</v>
       </c>
-      <c t="s" s="2" r="D30">
+      <c r="D37" s="2" t="s">
         <v>148</v>
       </c>
-      <c t="s" s="2" r="E30">
+      <c r="E37" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="31">
-      <c t="s" s="2" r="A31">
+      <c r="B38" s="1" t="s">
         <v>150</v>
       </c>
-      <c t="s" s="1" r="B31">
+      <c r="C38" s="2" t="s">
         <v>151</v>
       </c>
-      <c t="s" s="2" r="C31">
+      <c r="D38" s="2" t="s">
         <v>152</v>
       </c>
-      <c t="s" s="2" r="D31">
+      <c r="E38" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>153</v>
       </c>
-      <c t="s" s="2" r="E31">
+      <c r="B39" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="32">
-      <c t="s" s="2" r="A32">
+      <c r="C39" s="2" t="s">
         <v>155</v>
       </c>
-      <c t="s" s="1" r="B32">
+      <c r="D39" s="2" t="s">
         <v>156</v>
       </c>
-      <c t="s" s="2" r="C32">
+      <c r="E39" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>157</v>
       </c>
-      <c t="s" s="2" r="D32">
+      <c r="B40" s="1" t="s">
         <v>158</v>
       </c>
-      <c t="s" s="2" r="E32">
+      <c r="C40" s="2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="33">
-      <c t="s" s="2" r="A33">
+      <c r="D40" s="2" t="s">
         <v>160</v>
       </c>
-      <c t="s" s="1" r="B33">
+      <c r="E40" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
         <v>161</v>
       </c>
-      <c t="s" s="1" r="C33">
+      <c r="B41" s="1" t="s">
         <v>162</v>
       </c>
-      <c t="s" s="2" r="D33">
+      <c r="C41" s="2" t="s">
         <v>163</v>
       </c>
-      <c t="s" s="2" r="E33">
+      <c r="D41" s="2" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="34">
-      <c t="s" s="2" r="A34">
+      <c r="E41" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
         <v>165</v>
       </c>
-      <c t="s" s="1" r="B34">
+      <c r="B42" s="1" t="s">
         <v>166</v>
       </c>
-      <c t="s" s="1" r="C34">
+      <c r="C42" s="2" t="s">
         <v>167</v>
       </c>
-      <c t="s" s="2" r="D34">
+      <c r="D42" s="2" t="s">
         <v>168</v>
       </c>
-      <c t="s" s="2" r="E34">
+      <c r="E42" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="35">
-      <c t="s" s="2" r="A35">
+      <c r="B43" s="1" t="s">
         <v>170</v>
       </c>
-      <c t="s" s="1" r="B35">
+      <c r="C43" s="2" t="s">
         <v>171</v>
       </c>
-      <c t="s" s="1" r="C35">
+      <c r="D43" s="2" t="s">
         <v>172</v>
       </c>
-      <c t="s" s="2" r="D35">
+      <c r="E43" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
         <v>173</v>
       </c>
-      <c t="s" s="2" r="E35">
+      <c r="B44" s="1" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="36">
-      <c t="s" s="2" r="A36">
+      <c r="C44" s="2" t="s">
         <v>175</v>
       </c>
-      <c t="s" s="1" r="B36">
+      <c r="D44" s="2" t="s">
         <v>176</v>
       </c>
-      <c t="s" s="1" r="C36">
+      <c r="E44" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
         <v>177</v>
       </c>
-      <c t="s" s="2" r="D36">
+      <c r="B45" s="1" t="s">
         <v>178</v>
       </c>
-      <c t="s" s="2" r="E36">
+      <c r="C45" s="2" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="37">
-      <c t="s" s="2" r="A37">
+      <c r="D45" s="2" t="s">
         <v>180</v>
       </c>
-      <c t="s" s="1" r="B37">
+      <c r="E45" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
         <v>181</v>
       </c>
-      <c t="s" s="2" r="C37">
+      <c r="B46" s="1" t="s">
         <v>182</v>
       </c>
-      <c t="s" s="2" r="D37">
+      <c r="C46" s="2" t="s">
         <v>183</v>
       </c>
-      <c t="s" s="2" r="E37">
+      <c r="D46" s="2" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="38">
-      <c t="s" s="2" r="A38">
+      <c r="E46" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
         <v>185</v>
       </c>
-      <c t="s" s="1" r="B38">
+      <c r="B47" s="1" t="s">
         <v>186</v>
       </c>
-      <c t="s" s="2" r="C38">
+      <c r="C47" s="2" t="s">
         <v>187</v>
       </c>
-      <c t="s" s="2" r="D38">
+      <c r="D47" s="2" t="s">
         <v>188</v>
       </c>
-      <c t="s" s="2" r="E38">
+      <c r="E47" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="39">
-      <c t="s" s="2" r="A39">
+      <c r="B48" s="1" t="s">
         <v>190</v>
       </c>
-      <c t="s" s="1" r="B39">
+      <c r="C48" s="2" t="s">
         <v>191</v>
       </c>
-      <c t="s" s="2" r="C39">
+      <c r="D48" s="2" t="s">
         <v>192</v>
       </c>
-      <c t="s" s="2" r="D39">
+      <c r="E48" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>193</v>
       </c>
-      <c t="s" s="2" r="E39">
+      <c r="B49" s="1" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="40">
-      <c t="s" s="2" r="A40">
+      <c r="C49" s="2" t="s">
         <v>195</v>
       </c>
-      <c t="s" s="1" r="B40">
+      <c r="D49" s="2" t="s">
         <v>196</v>
       </c>
-      <c t="s" s="2" r="C40">
+      <c r="E49" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
         <v>197</v>
       </c>
-      <c t="s" s="2" r="D40">
+      <c r="B50" s="1" t="s">
         <v>198</v>
       </c>
-      <c t="s" s="2" r="E40">
+      <c r="C50" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="41">
-      <c t="s" s="2" r="A41">
+      <c r="D50" s="2" t="s">
         <v>200</v>
       </c>
-      <c t="s" s="1" r="B41">
+      <c r="E50" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
         <v>201</v>
       </c>
-      <c t="s" s="2" r="C41">
+      <c r="B51" s="1" t="s">
         <v>202</v>
       </c>
-      <c t="s" s="2" r="D41">
+      <c r="C51" s="1" t="s">
         <v>203</v>
       </c>
-      <c t="s" s="2" r="E41">
+      <c r="D51" s="2" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="42">
-      <c t="s" s="2" r="A42">
+      <c r="E51" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
         <v>205</v>
       </c>
-      <c t="s" s="1" r="B42">
+      <c r="B52" s="1" t="s">
         <v>206</v>
       </c>
-      <c t="s" s="2" r="C42">
+      <c r="C52" s="1" t="s">
         <v>207</v>
       </c>
-      <c t="s" s="2" r="D42">
+      <c r="D52" s="2" t="s">
         <v>208</v>
       </c>
-      <c t="s" s="2" r="E42">
+      <c r="E52" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="43">
-      <c t="s" s="2" r="A43">
+      <c r="B53" s="1" t="s">
         <v>210</v>
       </c>
-      <c t="s" s="1" r="B43">
+      <c r="C53" s="1" t="s">
         <v>211</v>
       </c>
-      <c t="s" s="2" r="C43">
+      <c r="D53" s="2" t="s">
         <v>212</v>
       </c>
-      <c t="s" s="2" r="D43">
+      <c r="E53" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
         <v>213</v>
       </c>
-      <c t="s" s="2" r="E43">
+      <c r="B54" s="1" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="44">
-      <c t="s" s="2" r="A44">
+      <c r="C54" s="1" t="s">
         <v>215</v>
       </c>
-      <c t="s" s="1" r="B44">
+      <c r="D54" s="2" t="s">
         <v>216</v>
       </c>
-      <c t="s" s="2" r="C44">
+      <c r="E54" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
         <v>217</v>
       </c>
-      <c t="s" s="2" r="D44">
+      <c r="B55" s="1" t="s">
         <v>218</v>
       </c>
-      <c t="s" s="2" r="E44">
+      <c r="C55" s="1" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="45">
-      <c t="s" s="2" r="A45">
+      <c r="D55" s="2" t="s">
         <v>220</v>
       </c>
-      <c t="s" s="1" r="B45">
+      <c r="E55" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
         <v>221</v>
       </c>
-      <c t="s" s="2" r="C45">
+      <c r="B56" s="1" t="s">
         <v>222</v>
       </c>
-      <c t="s" s="2" r="D45">
+      <c r="C56" s="1" t="s">
         <v>223</v>
       </c>
-      <c t="s" s="2" r="E45">
+      <c r="D56" s="2" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="46">
-      <c t="s" s="2" r="A46">
+      <c r="E56" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
         <v>225</v>
       </c>
-      <c t="s" s="1" r="B46">
+      <c r="B57" s="1" t="s">
         <v>226</v>
       </c>
-      <c t="s" s="2" r="C46">
+      <c r="C57" s="1" t="s">
         <v>227</v>
       </c>
-      <c t="s" s="2" r="D46">
+      <c r="D57" s="2" t="s">
         <v>228</v>
       </c>
-      <c t="s" s="2" r="E46">
+      <c r="E57" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="47">
-      <c t="s" s="2" r="A47">
+      <c r="B58" s="1" t="s">
         <v>230</v>
       </c>
-      <c t="s" s="1" r="B47">
+      <c r="C58" s="1" t="s">
         <v>231</v>
       </c>
-      <c t="s" s="2" r="C47">
+      <c r="D58" s="2" t="s">
         <v>232</v>
       </c>
-      <c t="s" s="2" r="D47">
+      <c r="E58" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
         <v>233</v>
       </c>
-      <c t="s" s="2" r="E47">
+      <c r="B59" s="1" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="48">
-      <c t="s" s="2" r="A48">
+      <c r="C59" s="1" t="s">
         <v>235</v>
       </c>
-      <c t="s" s="1" r="B48">
+      <c r="D59" s="2" t="s">
         <v>236</v>
       </c>
-      <c t="s" s="2" r="C48">
-        <v>237</v>
-      </c>
-      <c t="s" s="2" r="D48">
-        <v>238</v>
-      </c>
-      <c t="s" s="2" r="E48">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="49">
-      <c t="s" s="2" r="A49">
-        <v>240</v>
-      </c>
-      <c t="s" s="1" r="B49">
-        <v>241</v>
-      </c>
-      <c t="s" s="2" r="C49">
-        <v>242</v>
-      </c>
-      <c t="s" s="2" r="D49">
-        <v>243</v>
-      </c>
-      <c t="s" s="2" r="E49">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="50">
-      <c t="s" s="2" r="A50">
-        <v>245</v>
-      </c>
-      <c t="s" s="1" r="B50">
-        <v>246</v>
-      </c>
-      <c t="s" s="1" r="C50">
-        <v>247</v>
-      </c>
-      <c t="s" s="2" r="D50">
-        <v>248</v>
-      </c>
-      <c t="s" s="2" r="E50">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="51">
-      <c t="s" s="2" r="A51">
-        <v>250</v>
-      </c>
-      <c t="s" s="1" r="B51">
-        <v>251</v>
-      </c>
-      <c t="s" s="1" r="C51">
-        <v>252</v>
-      </c>
-      <c t="s" s="2" r="D51">
-        <v>253</v>
-      </c>
-      <c t="s" s="2" r="E51">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="52">
-      <c t="s" s="2" r="A52">
-        <v>255</v>
-      </c>
-      <c t="s" s="1" r="B52">
-        <v>256</v>
-      </c>
-      <c t="s" s="1" r="C52">
-        <v>257</v>
-      </c>
-      <c t="s" s="2" r="D52">
-        <v>258</v>
-      </c>
-      <c t="s" s="2" r="E52">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="53">
-      <c t="s" s="2" r="A53">
-        <v>260</v>
-      </c>
-      <c t="s" s="1" r="B53">
-        <v>261</v>
-      </c>
-      <c t="s" s="1" r="C53">
-        <v>262</v>
-      </c>
-      <c t="s" s="2" r="D53">
-        <v>263</v>
-      </c>
-      <c t="s" s="2" r="E53">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="54">
-      <c t="s" s="2" r="A54">
-        <v>265</v>
-      </c>
-      <c t="s" s="1" r="B54">
-        <v>266</v>
-      </c>
-      <c t="s" s="1" r="C54">
-        <v>267</v>
-      </c>
-      <c t="s" s="2" r="D54">
-        <v>268</v>
-      </c>
-      <c t="s" s="2" r="E54">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="55">
-      <c t="s" s="2" r="A55">
-        <v>270</v>
-      </c>
-      <c t="s" s="1" r="B55">
-        <v>271</v>
-      </c>
-      <c t="s" s="1" r="C55">
-        <v>272</v>
-      </c>
-      <c t="s" s="2" r="D55">
-        <v>273</v>
-      </c>
-      <c t="s" s="2" r="E55">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="56">
-      <c t="s" s="2" r="A56">
-        <v>275</v>
-      </c>
-      <c t="s" s="1" r="B56">
-        <v>276</v>
-      </c>
-      <c t="s" s="1" r="C56">
-        <v>277</v>
-      </c>
-      <c t="s" s="2" r="D56">
-        <v>278</v>
-      </c>
-      <c t="s" s="2" r="E56">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="57">
-      <c t="s" s="2" r="A57">
-        <v>280</v>
-      </c>
-      <c t="s" s="1" r="B57">
-        <v>281</v>
-      </c>
-      <c t="s" s="1" r="C57">
-        <v>282</v>
-      </c>
-      <c t="s" s="2" r="D57">
-        <v>283</v>
-      </c>
-      <c t="s" s="2" r="E57">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="58">
-      <c t="s" s="2" r="A58">
-        <v>285</v>
-      </c>
-      <c t="s" s="1" r="B58">
-        <v>286</v>
-      </c>
-      <c t="s" s="1" r="C58">
-        <v>287</v>
-      </c>
-      <c t="s" s="2" r="D58">
-        <v>288</v>
-      </c>
-      <c t="s" s="2" r="E58">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="59">
-      <c t="s" s="2" r="A59">
-        <v>290</v>
-      </c>
-      <c t="s" s="1" r="B59">
-        <v>291</v>
-      </c>
-      <c t="s" s="1" r="C59">
-        <v>292</v>
-      </c>
-      <c t="s" s="2" r="D59">
-        <v>293</v>
-      </c>
-      <c t="s" s="2" r="E59">
-        <v>294</v>
+      <c r="E59" s="3" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Data is now an Object. Updated imports and exports appropriately.
</commit_message>
<xml_diff>
--- a/working/providers/providers.xlsx
+++ b/working/providers/providers.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="238">
   <si>
     <t>PROVIDER_ID</t>
   </si>
@@ -727,10 +727,7 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>xlsx</t>
-  </si>
-  <si>
-    <t>xls</t>
+    <t>csv</t>
   </si>
 </sst>
 </file>
@@ -745,6 +742,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -774,11 +772,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1082,20 +1082,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="14.42578125" style="5"/>
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
     <col min="3" max="3" width="26.42578125" customWidth="1"/>
     <col min="4" max="4" width="26.28515625" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1111,8 +1112,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1124,12 +1125,12 @@
       <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1141,12 +1142,12 @@
       <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="E3" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1158,12 +1159,12 @@
       <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="E4" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1175,12 +1176,12 @@
       <c r="D5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="E5" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1192,12 +1193,12 @@
       <c r="D6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="E6" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1209,12 +1210,12 @@
       <c r="D7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="E7" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1226,12 +1227,12 @@
       <c r="D8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="E8" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1243,12 +1244,12 @@
       <c r="D9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="E9" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1260,12 +1261,12 @@
       <c r="D10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="E10" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1277,12 +1278,12 @@
       <c r="D11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="E11" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1294,12 +1295,12 @@
       <c r="D12" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="E12" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1311,12 +1312,12 @@
       <c r="D13" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="E13" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>53</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1328,12 +1329,12 @@
       <c r="D14" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="E14" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>57</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1345,12 +1346,12 @@
       <c r="D15" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="E15" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1362,12 +1363,12 @@
       <c r="D16" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="E16" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>65</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1379,12 +1380,12 @@
       <c r="D17" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="E17" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>69</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1396,12 +1397,12 @@
       <c r="D18" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="E18" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>73</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1413,12 +1414,12 @@
       <c r="D19" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="E19" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>77</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1430,12 +1431,12 @@
       <c r="D20" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="E20" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>81</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1447,12 +1448,12 @@
       <c r="D21" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="E21" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>85</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1464,12 +1465,12 @@
       <c r="D22" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="E22" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>89</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1481,12 +1482,12 @@
       <c r="D23" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="E23" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
         <v>93</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1498,12 +1499,12 @@
       <c r="D24" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="E24" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
         <v>97</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1515,12 +1516,12 @@
       <c r="D25" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="E25" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1532,12 +1533,12 @@
       <c r="D26" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="E26" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
         <v>105</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -1549,12 +1550,12 @@
       <c r="D27" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="E27" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
         <v>109</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1566,12 +1567,12 @@
       <c r="D28" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="E28" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
         <v>113</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1583,12 +1584,12 @@
       <c r="D29" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+      <c r="E29" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
         <v>117</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1600,12 +1601,12 @@
       <c r="D30" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+      <c r="E30" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
         <v>121</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1617,12 +1618,12 @@
       <c r="D31" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+      <c r="E31" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
         <v>125</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1634,12 +1635,12 @@
       <c r="D32" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
+      <c r="E32" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
         <v>129</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1651,12 +1652,12 @@
       <c r="D33" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+      <c r="E33" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
         <v>133</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1668,12 +1669,12 @@
       <c r="D34" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+      <c r="E34" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
         <v>137</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1685,12 +1686,12 @@
       <c r="D35" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E35" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
+      <c r="E35" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
         <v>141</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1702,12 +1703,12 @@
       <c r="D36" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+      <c r="E36" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
         <v>145</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -1719,12 +1720,12 @@
       <c r="D37" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E37" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
+      <c r="E37" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
         <v>149</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1736,12 +1737,12 @@
       <c r="D38" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E38" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
+      <c r="E38" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
         <v>153</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -1753,12 +1754,12 @@
       <c r="D39" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="E39" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
+      <c r="E39" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
         <v>157</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -1770,12 +1771,12 @@
       <c r="D40" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="E40" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
+      <c r="E40" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
         <v>161</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -1787,12 +1788,12 @@
       <c r="D41" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E41" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
+      <c r="E41" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
         <v>165</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -1804,12 +1805,12 @@
       <c r="D42" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E42" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
+      <c r="E42" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
         <v>169</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -1821,12 +1822,12 @@
       <c r="D43" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E43" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
+      <c r="E43" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
         <v>173</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -1838,12 +1839,12 @@
       <c r="D44" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
+      <c r="E44" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
         <v>177</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -1855,12 +1856,12 @@
       <c r="D45" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E45" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
+      <c r="E45" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
         <v>181</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -1872,12 +1873,12 @@
       <c r="D46" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E46" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
+      <c r="E46" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
         <v>185</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -1889,12 +1890,12 @@
       <c r="D47" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E47" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
+      <c r="E47" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
         <v>189</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -1906,12 +1907,12 @@
       <c r="D48" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="E48" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
+      <c r="E48" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
         <v>193</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -1923,12 +1924,12 @@
       <c r="D49" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="E49" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
+      <c r="E49" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
         <v>197</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -1940,12 +1941,12 @@
       <c r="D50" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E50" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
+      <c r="E50" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
         <v>201</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -1957,12 +1958,12 @@
       <c r="D51" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="E51" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
+      <c r="E51" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A52" s="4" t="s">
         <v>205</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -1974,12 +1975,12 @@
       <c r="D52" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="E52" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
+      <c r="E52" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
         <v>209</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -1991,12 +1992,12 @@
       <c r="D53" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="E53" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
+      <c r="E53" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A54" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -2008,12 +2009,12 @@
       <c r="D54" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="E54" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
+      <c r="E54" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="s">
         <v>217</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -2025,12 +2026,12 @@
       <c r="D55" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="E55" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
+      <c r="E55" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
         <v>221</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -2042,12 +2043,12 @@
       <c r="D56" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="E56" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
+      <c r="E56" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A57" s="4" t="s">
         <v>225</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -2059,12 +2060,12 @@
       <c r="D57" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="E57" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
+      <c r="E57" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
         <v>229</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -2076,12 +2077,12 @@
       <c r="D58" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="E58" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
+      <c r="E58" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A59" s="4" t="s">
         <v>233</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -2093,7 +2094,7 @@
       <c r="D59" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="E59" s="2" t="s">
         <v>237</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating schema object structure to assist with defining validation rules. updating xml ingest logic for updated object structure.
</commit_message>
<xml_diff>
--- a/working/providers/providers.xlsx
+++ b/working/providers/providers.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="870" yWindow="900" windowWidth="18780" windowHeight="6570"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$A$1:$E$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$59</definedName>
   </definedNames>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="238">
   <si>
     <t>PROVIDER_ID</t>
   </si>
@@ -42,9 +46,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>005</t>
   </si>
   <si>
@@ -57,9 +58,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>005</t>
   </si>
   <si>
@@ -72,9 +70,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>005</t>
   </si>
   <si>
@@ -87,9 +82,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>003</t>
   </si>
   <si>
@@ -102,9 +94,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>003</t>
   </si>
   <si>
@@ -117,9 +106,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>003</t>
   </si>
   <si>
@@ -132,9 +118,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>003</t>
   </si>
   <si>
@@ -147,9 +130,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>003</t>
   </si>
   <si>
@@ -162,9 +142,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>003</t>
   </si>
   <si>
@@ -177,9 +154,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>003</t>
   </si>
   <si>
@@ -192,9 +166,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>003</t>
   </si>
   <si>
@@ -207,9 +178,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>003</t>
   </si>
   <si>
@@ -222,9 +190,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>003</t>
   </si>
   <si>
@@ -237,9 +202,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>004</t>
   </si>
   <si>
@@ -252,9 +214,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>004</t>
   </si>
   <si>
@@ -267,9 +226,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>004</t>
   </si>
   <si>
@@ -282,9 +238,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>004</t>
   </si>
   <si>
@@ -297,9 +250,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>004</t>
   </si>
   <si>
@@ -312,9 +262,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>004</t>
   </si>
   <si>
@@ -327,9 +274,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>004</t>
   </si>
   <si>
@@ -342,9 +286,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>004</t>
   </si>
   <si>
@@ -357,9 +298,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>004</t>
   </si>
   <si>
@@ -372,9 +310,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>004</t>
   </si>
   <si>
@@ -387,9 +322,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>004</t>
   </si>
   <si>
@@ -402,9 +334,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>004</t>
   </si>
   <si>
@@ -417,9 +346,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>004</t>
   </si>
   <si>
@@ -432,9 +358,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -447,9 +370,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -462,9 +382,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -477,9 +394,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -492,9 +406,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -507,9 +418,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -522,9 +430,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -537,9 +442,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -552,9 +454,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -567,9 +466,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -582,9 +478,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -597,9 +490,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -612,9 +502,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -627,9 +514,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -642,9 +526,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -657,9 +538,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -672,9 +550,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -687,9 +562,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>002</t>
   </si>
   <si>
@@ -702,9 +574,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -717,9 +586,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -732,9 +598,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -747,9 +610,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -762,9 +622,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -777,9 +634,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -792,9 +646,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -807,9 +658,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -822,9 +670,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -837,9 +682,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -852,9 +694,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -867,9 +706,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>006</t>
   </si>
   <si>
@@ -882,9 +718,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>006</t>
   </si>
   <si>
@@ -897,26 +730,29 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
+    <t>xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
@@ -932,1048 +768,1337 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
-    <xf fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1"/>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
-      <alignment/>
-    </xf>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E59"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" customWidth="1" max="2" width="22.29"/>
-    <col min="3" customWidth="1" max="3" width="26.43"/>
-    <col min="4" customWidth="1" max="4" width="26.29"/>
-    <col min="5" customWidth="1" max="5" width="23.0"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c t="s" s="1" r="A1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c t="s" s="1" r="B1">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c t="s" s="1" r="C1">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="2" r="D1">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c t="s" s="2" r="E1">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c t="s" s="2" r="A2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c t="s" s="1" r="B2">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c t="s" s="1" r="C2">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="2" r="D2">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c t="s" s="2" r="E2">
+      <c r="E2" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3">
-      <c t="s" s="2" r="A3">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c t="s" s="1" r="B3">
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c t="s" s="1" r="C3">
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c t="s" s="2" r="D3">
+      <c r="E3" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c t="s" s="2" r="E3">
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4">
-      <c t="s" s="2" r="A4">
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c t="s" s="1" r="B4">
+      <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c t="s" s="1" r="C4">
+      <c r="E4" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
-      <c t="s" s="2" r="D4">
+      <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c t="s" s="2" r="E4">
+      <c r="C5" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5">
-      <c t="s" s="2" r="A5">
+      <c r="D5" s="2" t="s">
         <v>20</v>
       </c>
-      <c t="s" s="1" r="B5">
+      <c r="E5" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
-      <c t="s" s="1" r="C5">
+      <c r="B6" s="1" t="s">
         <v>22</v>
       </c>
-      <c t="s" s="2" r="D5">
+      <c r="C6" s="1" t="s">
         <v>23</v>
       </c>
-      <c t="s" s="2" r="E5">
+      <c r="D6" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6">
-      <c t="s" s="2" r="A6">
+      <c r="E6" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c t="s" s="1" r="B6">
+      <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
-      <c t="s" s="1" r="C6">
+      <c r="C7" s="1" t="s">
         <v>27</v>
       </c>
-      <c t="s" s="2" r="D6">
+      <c r="D7" s="2" t="s">
         <v>28</v>
       </c>
-      <c t="s" s="2" r="E6">
+      <c r="E7" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7">
-      <c t="s" s="2" r="A7">
+      <c r="B8" s="1" t="s">
         <v>30</v>
       </c>
-      <c t="s" s="1" r="B7">
+      <c r="C8" s="1" t="s">
         <v>31</v>
       </c>
-      <c t="s" s="1" r="C7">
+      <c r="D8" s="2" t="s">
         <v>32</v>
       </c>
-      <c t="s" s="2" r="D7">
+      <c r="E8" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>33</v>
       </c>
-      <c t="s" s="2" r="E7">
+      <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8">
-      <c t="s" s="2" r="A8">
+      <c r="C9" s="1" t="s">
         <v>35</v>
       </c>
-      <c t="s" s="1" r="B8">
+      <c r="D9" s="2" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="1" r="C8">
+      <c r="E9" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
-      <c t="s" s="2" r="D8">
+      <c r="B10" s="1" t="s">
         <v>38</v>
       </c>
-      <c t="s" s="2" r="E8">
+      <c r="C10" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="9">
-      <c t="s" s="2" r="A9">
+      <c r="D10" s="2" t="s">
         <v>40</v>
       </c>
-      <c t="s" s="1" r="B9">
+      <c r="E10" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>41</v>
       </c>
-      <c t="s" s="1" r="C9">
+      <c r="B11" s="1" t="s">
         <v>42</v>
       </c>
-      <c t="s" s="2" r="D9">
+      <c r="C11" s="1" t="s">
         <v>43</v>
       </c>
-      <c t="s" s="2" r="E9">
+      <c r="D11" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="10">
-      <c t="s" s="2" r="A10">
+      <c r="E11" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>45</v>
       </c>
-      <c t="s" s="1" r="B10">
+      <c r="B12" s="1" t="s">
         <v>46</v>
       </c>
-      <c t="s" s="1" r="C10">
+      <c r="C12" s="1" t="s">
         <v>47</v>
       </c>
-      <c t="s" s="2" r="D10">
+      <c r="D12" s="2" t="s">
         <v>48</v>
       </c>
-      <c t="s" s="2" r="E10">
+      <c r="E12" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="11">
-      <c t="s" s="2" r="A11">
+      <c r="B13" s="1" t="s">
         <v>50</v>
       </c>
-      <c t="s" s="1" r="B11">
+      <c r="C13" s="1" t="s">
         <v>51</v>
       </c>
-      <c t="s" s="1" r="C11">
+      <c r="D13" s="2" t="s">
         <v>52</v>
       </c>
-      <c t="s" s="2" r="D11">
+      <c r="E13" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>53</v>
       </c>
-      <c t="s" s="2" r="E11">
+      <c r="B14" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="12">
-      <c t="s" s="2" r="A12">
+      <c r="C14" s="1" t="s">
         <v>55</v>
       </c>
-      <c t="s" s="1" r="B12">
+      <c r="D14" s="2" t="s">
         <v>56</v>
       </c>
-      <c t="s" s="1" r="C12">
+      <c r="E14" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>57</v>
       </c>
-      <c t="s" s="2" r="D12">
+      <c r="B15" s="1" t="s">
         <v>58</v>
       </c>
-      <c t="s" s="2" r="E12">
+      <c r="C15" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="13">
-      <c t="s" s="2" r="A13">
+      <c r="D15" s="2" t="s">
         <v>60</v>
       </c>
-      <c t="s" s="1" r="B13">
+      <c r="E15" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>61</v>
       </c>
-      <c t="s" s="1" r="C13">
+      <c r="B16" s="1" t="s">
         <v>62</v>
       </c>
-      <c t="s" s="2" r="D13">
+      <c r="C16" s="2" t="s">
         <v>63</v>
       </c>
-      <c t="s" s="2" r="E13">
+      <c r="D16" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="14">
-      <c t="s" s="2" r="A14">
+      <c r="E16" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>65</v>
       </c>
-      <c t="s" s="1" r="B14">
+      <c r="B17" s="1" t="s">
         <v>66</v>
       </c>
-      <c t="s" s="1" r="C14">
+      <c r="C17" s="2" t="s">
         <v>67</v>
       </c>
-      <c t="s" s="2" r="D14">
+      <c r="D17" s="2" t="s">
         <v>68</v>
       </c>
-      <c t="s" s="2" r="E14">
+      <c r="E17" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="15">
-      <c t="s" s="2" r="A15">
+      <c r="B18" s="1" t="s">
         <v>70</v>
       </c>
-      <c t="s" s="1" r="B15">
+      <c r="C18" s="2" t="s">
         <v>71</v>
       </c>
-      <c t="s" s="1" r="C15">
+      <c r="D18" s="2" t="s">
         <v>72</v>
       </c>
-      <c t="s" s="2" r="D15">
+      <c r="E18" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>73</v>
       </c>
-      <c t="s" s="2" r="E15">
+      <c r="B19" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="16">
-      <c t="s" s="2" r="A16">
+      <c r="C19" s="2" t="s">
         <v>75</v>
       </c>
-      <c t="s" s="1" r="B16">
+      <c r="D19" s="2" t="s">
         <v>76</v>
       </c>
-      <c t="s" s="2" r="C16">
+      <c r="E19" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>77</v>
       </c>
-      <c t="s" s="2" r="D16">
+      <c r="B20" s="1" t="s">
         <v>78</v>
       </c>
-      <c t="s" s="2" r="E16">
+      <c r="C20" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="17">
-      <c t="s" s="2" r="A17">
+      <c r="D20" s="2" t="s">
         <v>80</v>
       </c>
-      <c t="s" s="1" r="B17">
+      <c r="E20" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>81</v>
       </c>
-      <c t="s" s="2" r="C17">
+      <c r="B21" s="1" t="s">
         <v>82</v>
       </c>
-      <c t="s" s="2" r="D17">
+      <c r="C21" s="2" t="s">
         <v>83</v>
       </c>
-      <c t="s" s="2" r="E17">
+      <c r="D21" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="18">
-      <c t="s" s="2" r="A18">
+      <c r="E21" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>85</v>
       </c>
-      <c t="s" s="1" r="B18">
+      <c r="B22" s="1" t="s">
         <v>86</v>
       </c>
-      <c t="s" s="2" r="C18">
+      <c r="C22" s="2" t="s">
         <v>87</v>
       </c>
-      <c t="s" s="2" r="D18">
+      <c r="D22" s="2" t="s">
         <v>88</v>
       </c>
-      <c t="s" s="2" r="E18">
+      <c r="E22" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="19">
-      <c t="s" s="2" r="A19">
+      <c r="B23" s="1" t="s">
         <v>90</v>
       </c>
-      <c t="s" s="1" r="B19">
+      <c r="C23" s="2" t="s">
         <v>91</v>
       </c>
-      <c t="s" s="2" r="C19">
+      <c r="D23" s="2" t="s">
         <v>92</v>
       </c>
-      <c t="s" s="2" r="D19">
+      <c r="E23" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>93</v>
       </c>
-      <c t="s" s="2" r="E19">
+      <c r="B24" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="20">
-      <c t="s" s="2" r="A20">
+      <c r="C24" s="2" t="s">
         <v>95</v>
       </c>
-      <c t="s" s="1" r="B20">
+      <c r="D24" s="2" t="s">
         <v>96</v>
       </c>
-      <c t="s" s="2" r="C20">
+      <c r="E24" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>97</v>
       </c>
-      <c t="s" s="2" r="D20">
+      <c r="B25" s="1" t="s">
         <v>98</v>
       </c>
-      <c t="s" s="2" r="E20">
+      <c r="C25" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="21">
-      <c t="s" s="2" r="A21">
+      <c r="D25" s="2" t="s">
         <v>100</v>
       </c>
-      <c t="s" s="1" r="B21">
+      <c r="E25" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>101</v>
       </c>
-      <c t="s" s="2" r="C21">
+      <c r="B26" s="1" t="s">
         <v>102</v>
       </c>
-      <c t="s" s="2" r="D21">
+      <c r="C26" s="2" t="s">
         <v>103</v>
       </c>
-      <c t="s" s="2" r="E21">
+      <c r="D26" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="22">
-      <c t="s" s="2" r="A22">
+      <c r="E26" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>105</v>
       </c>
-      <c t="s" s="1" r="B22">
+      <c r="B27" s="1" t="s">
         <v>106</v>
       </c>
-      <c t="s" s="2" r="C22">
+      <c r="C27" s="2" t="s">
         <v>107</v>
       </c>
-      <c t="s" s="2" r="D22">
+      <c r="D27" s="2" t="s">
         <v>108</v>
       </c>
-      <c t="s" s="2" r="E22">
+      <c r="E27" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="23">
-      <c t="s" s="2" r="A23">
+      <c r="B28" s="1" t="s">
         <v>110</v>
       </c>
-      <c t="s" s="1" r="B23">
+      <c r="C28" s="2" t="s">
         <v>111</v>
       </c>
-      <c t="s" s="2" r="C23">
+      <c r="D28" s="2" t="s">
         <v>112</v>
       </c>
-      <c t="s" s="2" r="D23">
+      <c r="E28" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>113</v>
       </c>
-      <c t="s" s="2" r="E23">
+      <c r="B29" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="24">
-      <c t="s" s="2" r="A24">
+      <c r="C29" s="2" t="s">
         <v>115</v>
       </c>
-      <c t="s" s="1" r="B24">
+      <c r="D29" s="2" t="s">
         <v>116</v>
       </c>
-      <c t="s" s="2" r="C24">
+      <c r="E29" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>117</v>
       </c>
-      <c t="s" s="2" r="D24">
+      <c r="B30" s="1" t="s">
         <v>118</v>
       </c>
-      <c t="s" s="2" r="E24">
+      <c r="C30" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="25">
-      <c t="s" s="2" r="A25">
+      <c r="D30" s="2" t="s">
         <v>120</v>
       </c>
-      <c t="s" s="1" r="B25">
+      <c r="E30" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>121</v>
       </c>
-      <c t="s" s="2" r="C25">
+      <c r="B31" s="1" t="s">
         <v>122</v>
       </c>
-      <c t="s" s="2" r="D25">
+      <c r="C31" s="2" t="s">
         <v>123</v>
       </c>
-      <c t="s" s="2" r="E25">
+      <c r="D31" s="2" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="26">
-      <c t="s" s="2" r="A26">
+      <c r="E31" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>125</v>
       </c>
-      <c t="s" s="1" r="B26">
+      <c r="B32" s="1" t="s">
         <v>126</v>
       </c>
-      <c t="s" s="2" r="C26">
+      <c r="C32" s="2" t="s">
         <v>127</v>
       </c>
-      <c t="s" s="2" r="D26">
+      <c r="D32" s="2" t="s">
         <v>128</v>
       </c>
-      <c t="s" s="2" r="E26">
+      <c r="E32" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="27">
-      <c t="s" s="2" r="A27">
+      <c r="B33" s="1" t="s">
         <v>130</v>
       </c>
-      <c t="s" s="1" r="B27">
+      <c r="C33" s="2" t="s">
         <v>131</v>
       </c>
-      <c t="s" s="2" r="C27">
+      <c r="D33" s="2" t="s">
         <v>132</v>
       </c>
-      <c t="s" s="2" r="D27">
+      <c r="E33" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
         <v>133</v>
       </c>
-      <c t="s" s="2" r="E27">
+      <c r="B34" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="28">
-      <c t="s" s="2" r="A28">
+      <c r="C34" s="2" t="s">
         <v>135</v>
       </c>
-      <c t="s" s="1" r="B28">
+      <c r="D34" s="2" t="s">
         <v>136</v>
       </c>
-      <c t="s" s="2" r="C28">
+      <c r="E34" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>137</v>
       </c>
-      <c t="s" s="2" r="D28">
+      <c r="B35" s="1" t="s">
         <v>138</v>
       </c>
-      <c t="s" s="2" r="E28">
+      <c r="C35" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="29">
-      <c t="s" s="2" r="A29">
+      <c r="D35" s="2" t="s">
         <v>140</v>
       </c>
-      <c t="s" s="1" r="B29">
+      <c r="E35" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>141</v>
       </c>
-      <c t="s" s="2" r="C29">
+      <c r="B36" s="1" t="s">
         <v>142</v>
       </c>
-      <c t="s" s="2" r="D29">
+      <c r="C36" s="2" t="s">
         <v>143</v>
       </c>
-      <c t="s" s="2" r="E29">
+      <c r="D36" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="30">
-      <c t="s" s="2" r="A30">
+      <c r="E36" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>145</v>
       </c>
-      <c t="s" s="1" r="B30">
+      <c r="B37" s="1" t="s">
         <v>146</v>
       </c>
-      <c t="s" s="2" r="C30">
+      <c r="C37" s="2" t="s">
         <v>147</v>
       </c>
-      <c t="s" s="2" r="D30">
+      <c r="D37" s="2" t="s">
         <v>148</v>
       </c>
-      <c t="s" s="2" r="E30">
+      <c r="E37" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="31">
-      <c t="s" s="2" r="A31">
+      <c r="B38" s="1" t="s">
         <v>150</v>
       </c>
-      <c t="s" s="1" r="B31">
+      <c r="C38" s="2" t="s">
         <v>151</v>
       </c>
-      <c t="s" s="2" r="C31">
+      <c r="D38" s="2" t="s">
         <v>152</v>
       </c>
-      <c t="s" s="2" r="D31">
+      <c r="E38" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>153</v>
       </c>
-      <c t="s" s="2" r="E31">
+      <c r="B39" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="32">
-      <c t="s" s="2" r="A32">
+      <c r="C39" s="2" t="s">
         <v>155</v>
       </c>
-      <c t="s" s="1" r="B32">
+      <c r="D39" s="2" t="s">
         <v>156</v>
       </c>
-      <c t="s" s="2" r="C32">
+      <c r="E39" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>157</v>
       </c>
-      <c t="s" s="2" r="D32">
+      <c r="B40" s="1" t="s">
         <v>158</v>
       </c>
-      <c t="s" s="2" r="E32">
+      <c r="C40" s="2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="33">
-      <c t="s" s="2" r="A33">
+      <c r="D40" s="2" t="s">
         <v>160</v>
       </c>
-      <c t="s" s="1" r="B33">
+      <c r="E40" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
         <v>161</v>
       </c>
-      <c t="s" s="2" r="C33">
+      <c r="B41" s="1" t="s">
         <v>162</v>
       </c>
-      <c t="s" s="2" r="D33">
+      <c r="C41" s="2" t="s">
         <v>163</v>
       </c>
-      <c t="s" s="2" r="E33">
+      <c r="D41" s="2" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="34">
-      <c t="s" s="2" r="A34">
+      <c r="E41" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
         <v>165</v>
       </c>
-      <c t="s" s="1" r="B34">
+      <c r="B42" s="1" t="s">
         <v>166</v>
       </c>
-      <c t="s" s="2" r="C34">
+      <c r="C42" s="2" t="s">
         <v>167</v>
       </c>
-      <c t="s" s="2" r="D34">
+      <c r="D42" s="2" t="s">
         <v>168</v>
       </c>
-      <c t="s" s="2" r="E34">
+      <c r="E42" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="35">
-      <c t="s" s="2" r="A35">
+      <c r="B43" s="1" t="s">
         <v>170</v>
       </c>
-      <c t="s" s="1" r="B35">
+      <c r="C43" s="2" t="s">
         <v>171</v>
       </c>
-      <c t="s" s="2" r="C35">
+      <c r="D43" s="2" t="s">
         <v>172</v>
       </c>
-      <c t="s" s="2" r="D35">
+      <c r="E43" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
         <v>173</v>
       </c>
-      <c t="s" s="2" r="E35">
+      <c r="B44" s="1" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="36">
-      <c t="s" s="2" r="A36">
+      <c r="C44" s="2" t="s">
         <v>175</v>
       </c>
-      <c t="s" s="1" r="B36">
+      <c r="D44" s="2" t="s">
         <v>176</v>
       </c>
-      <c t="s" s="2" r="C36">
+      <c r="E44" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
         <v>177</v>
       </c>
-      <c t="s" s="2" r="D36">
+      <c r="B45" s="1" t="s">
         <v>178</v>
       </c>
-      <c t="s" s="2" r="E36">
+      <c r="C45" s="2" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="37">
-      <c t="s" s="2" r="A37">
+      <c r="D45" s="2" t="s">
         <v>180</v>
       </c>
-      <c t="s" s="1" r="B37">
+      <c r="E45" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
         <v>181</v>
       </c>
-      <c t="s" s="2" r="C37">
+      <c r="B46" s="1" t="s">
         <v>182</v>
       </c>
-      <c t="s" s="2" r="D37">
+      <c r="C46" s="2" t="s">
         <v>183</v>
       </c>
-      <c t="s" s="2" r="E37">
+      <c r="D46" s="2" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="38">
-      <c t="s" s="2" r="A38">
+      <c r="E46" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
         <v>185</v>
       </c>
-      <c t="s" s="1" r="B38">
+      <c r="B47" s="1" t="s">
         <v>186</v>
       </c>
-      <c t="s" s="2" r="C38">
+      <c r="C47" s="2" t="s">
         <v>187</v>
       </c>
-      <c t="s" s="2" r="D38">
+      <c r="D47" s="2" t="s">
         <v>188</v>
       </c>
-      <c t="s" s="2" r="E38">
+      <c r="E47" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="39">
-      <c t="s" s="2" r="A39">
+      <c r="B48" s="1" t="s">
         <v>190</v>
       </c>
-      <c t="s" s="1" r="B39">
+      <c r="C48" s="2" t="s">
         <v>191</v>
       </c>
-      <c t="s" s="2" r="C39">
+      <c r="D48" s="2" t="s">
         <v>192</v>
       </c>
-      <c t="s" s="2" r="D39">
+      <c r="E48" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>193</v>
       </c>
-      <c t="s" s="2" r="E39">
+      <c r="B49" s="1" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="40">
-      <c t="s" s="2" r="A40">
+      <c r="C49" s="2" t="s">
         <v>195</v>
       </c>
-      <c t="s" s="1" r="B40">
+      <c r="D49" s="2" t="s">
         <v>196</v>
       </c>
-      <c t="s" s="2" r="C40">
+      <c r="E49" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
         <v>197</v>
       </c>
-      <c t="s" s="2" r="D40">
+      <c r="B50" s="1" t="s">
         <v>198</v>
       </c>
-      <c t="s" s="2" r="E40">
+      <c r="C50" s="2" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="41">
-      <c t="s" s="2" r="A41">
+      <c r="D50" s="2" t="s">
         <v>200</v>
       </c>
-      <c t="s" s="1" r="B41">
+      <c r="E50" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
         <v>201</v>
       </c>
-      <c t="s" s="2" r="C41">
+      <c r="B51" s="1" t="s">
         <v>202</v>
       </c>
-      <c t="s" s="2" r="D41">
+      <c r="C51" s="2" t="s">
         <v>203</v>
       </c>
-      <c t="s" s="2" r="E41">
+      <c r="D51" s="2" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="42">
-      <c t="s" s="2" r="A42">
+      <c r="E51" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
         <v>205</v>
       </c>
-      <c t="s" s="1" r="B42">
+      <c r="B52" s="1" t="s">
         <v>206</v>
       </c>
-      <c t="s" s="2" r="C42">
+      <c r="C52" s="2" t="s">
         <v>207</v>
       </c>
-      <c t="s" s="2" r="D42">
+      <c r="D52" s="2" t="s">
         <v>208</v>
       </c>
-      <c t="s" s="2" r="E42">
+      <c r="E52" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="43">
-      <c t="s" s="2" r="A43">
+      <c r="B53" s="1" t="s">
         <v>210</v>
       </c>
-      <c t="s" s="1" r="B43">
+      <c r="C53" s="2" t="s">
         <v>211</v>
       </c>
-      <c t="s" s="2" r="C43">
+      <c r="D53" s="2" t="s">
         <v>212</v>
       </c>
-      <c t="s" s="2" r="D43">
+      <c r="E53" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
         <v>213</v>
       </c>
-      <c t="s" s="2" r="E43">
+      <c r="B54" s="1" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="44">
-      <c t="s" s="2" r="A44">
+      <c r="C54" s="2" t="s">
         <v>215</v>
       </c>
-      <c t="s" s="1" r="B44">
+      <c r="D54" s="2" t="s">
         <v>216</v>
       </c>
-      <c t="s" s="2" r="C44">
+      <c r="E54" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
         <v>217</v>
       </c>
-      <c t="s" s="2" r="D44">
+      <c r="B55" s="1" t="s">
         <v>218</v>
       </c>
-      <c t="s" s="2" r="E44">
+      <c r="C55" s="2" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="45">
-      <c t="s" s="2" r="A45">
+      <c r="D55" s="2" t="s">
         <v>220</v>
       </c>
-      <c t="s" s="1" r="B45">
+      <c r="E55" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
         <v>221</v>
       </c>
-      <c t="s" s="2" r="C45">
+      <c r="B56" s="1" t="s">
         <v>222</v>
       </c>
-      <c t="s" s="2" r="D45">
+      <c r="C56" s="2" t="s">
         <v>223</v>
       </c>
-      <c t="s" s="2" r="E45">
+      <c r="D56" s="2" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="46">
-      <c t="s" s="2" r="A46">
+      <c r="E56" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
         <v>225</v>
       </c>
-      <c t="s" s="1" r="B46">
+      <c r="B57" s="1" t="s">
         <v>226</v>
       </c>
-      <c t="s" s="2" r="C46">
+      <c r="C57" s="2" t="s">
         <v>227</v>
       </c>
-      <c t="s" s="2" r="D46">
+      <c r="D57" s="2" t="s">
         <v>228</v>
       </c>
-      <c t="s" s="2" r="E46">
+      <c r="E57" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="47">
-      <c t="s" s="2" r="A47">
+      <c r="B58" s="1" t="s">
         <v>230</v>
       </c>
-      <c t="s" s="1" r="B47">
+      <c r="C58" s="2" t="s">
         <v>231</v>
       </c>
-      <c t="s" s="2" r="C47">
+      <c r="D58" s="2" t="s">
         <v>232</v>
       </c>
-      <c t="s" s="2" r="D47">
+      <c r="E58" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
         <v>233</v>
       </c>
-      <c t="s" s="2" r="E47">
+      <c r="B59" s="1" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="48">
-      <c t="s" s="2" r="A48">
+      <c r="C59" s="2" t="s">
         <v>235</v>
       </c>
-      <c t="s" s="1" r="B48">
+      <c r="D59" s="2" t="s">
         <v>236</v>
       </c>
-      <c t="s" s="2" r="C48">
-        <v>237</v>
-      </c>
-      <c t="s" s="2" r="D48">
-        <v>238</v>
-      </c>
-      <c t="s" s="2" r="E48">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="49">
-      <c t="s" s="2" r="A49">
-        <v>240</v>
-      </c>
-      <c t="s" s="1" r="B49">
-        <v>241</v>
-      </c>
-      <c t="s" s="2" r="C49">
-        <v>242</v>
-      </c>
-      <c t="s" s="2" r="D49">
-        <v>243</v>
-      </c>
-      <c t="s" s="2" r="E49">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="50">
-      <c t="s" s="2" r="A50">
-        <v>245</v>
-      </c>
-      <c t="s" s="1" r="B50">
-        <v>246</v>
-      </c>
-      <c t="s" s="2" r="C50">
-        <v>247</v>
-      </c>
-      <c t="s" s="2" r="D50">
-        <v>248</v>
-      </c>
-      <c t="s" s="2" r="E50">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="51">
-      <c t="s" s="2" r="A51">
-        <v>250</v>
-      </c>
-      <c t="s" s="1" r="B51">
-        <v>251</v>
-      </c>
-      <c t="s" s="2" r="C51">
-        <v>252</v>
-      </c>
-      <c t="s" s="2" r="D51">
-        <v>253</v>
-      </c>
-      <c t="s" s="2" r="E51">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="52">
-      <c t="s" s="2" r="A52">
-        <v>255</v>
-      </c>
-      <c t="s" s="1" r="B52">
-        <v>256</v>
-      </c>
-      <c t="s" s="2" r="C52">
-        <v>257</v>
-      </c>
-      <c t="s" s="2" r="D52">
-        <v>258</v>
-      </c>
-      <c t="s" s="2" r="E52">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="53">
-      <c t="s" s="2" r="A53">
-        <v>260</v>
-      </c>
-      <c t="s" s="1" r="B53">
-        <v>261</v>
-      </c>
-      <c t="s" s="2" r="C53">
-        <v>262</v>
-      </c>
-      <c t="s" s="2" r="D53">
-        <v>263</v>
-      </c>
-      <c t="s" s="2" r="E53">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="54">
-      <c t="s" s="2" r="A54">
-        <v>265</v>
-      </c>
-      <c t="s" s="1" r="B54">
-        <v>266</v>
-      </c>
-      <c t="s" s="2" r="C54">
-        <v>267</v>
-      </c>
-      <c t="s" s="2" r="D54">
-        <v>268</v>
-      </c>
-      <c t="s" s="2" r="E54">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="55">
-      <c t="s" s="2" r="A55">
-        <v>270</v>
-      </c>
-      <c t="s" s="1" r="B55">
-        <v>271</v>
-      </c>
-      <c t="s" s="2" r="C55">
-        <v>272</v>
-      </c>
-      <c t="s" s="2" r="D55">
-        <v>273</v>
-      </c>
-      <c t="s" s="2" r="E55">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="56">
-      <c t="s" s="2" r="A56">
-        <v>275</v>
-      </c>
-      <c t="s" s="1" r="B56">
-        <v>276</v>
-      </c>
-      <c t="s" s="2" r="C56">
-        <v>277</v>
-      </c>
-      <c t="s" s="2" r="D56">
-        <v>278</v>
-      </c>
-      <c t="s" s="2" r="E56">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="57">
-      <c t="s" s="2" r="A57">
-        <v>280</v>
-      </c>
-      <c t="s" s="1" r="B57">
-        <v>281</v>
-      </c>
-      <c t="s" s="2" r="C57">
-        <v>282</v>
-      </c>
-      <c t="s" s="2" r="D57">
-        <v>283</v>
-      </c>
-      <c t="s" s="2" r="E57">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="58">
-      <c t="s" s="2" r="A58">
-        <v>285</v>
-      </c>
-      <c t="s" s="1" r="B58">
-        <v>286</v>
-      </c>
-      <c t="s" s="2" r="C58">
-        <v>287</v>
-      </c>
-      <c t="s" s="2" r="D58">
-        <v>288</v>
-      </c>
-      <c t="s" s="2" r="E58">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="59">
-      <c t="s" s="2" r="A59">
-        <v>290</v>
-      </c>
-      <c t="s" s="1" r="B59">
-        <v>291</v>
-      </c>
-      <c t="s" s="2" r="C59">
-        <v>292</v>
-      </c>
-      <c t="s" s="2" r="D59">
-        <v>293</v>
-      </c>
-      <c t="s" s="2" r="E59">
-        <v>294</v>
+      <c r="E59" s="3" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$E$59"/>
-  <drawing r:id="rId1"/>
+  <autoFilter ref="A1:E59"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updating providers methodology to match load-then-validate as well as the Java Strategy pattern
</commit_message>
<xml_diff>
--- a/working/providers/providers.xlsx
+++ b/working/providers/providers.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="239">
   <si>
     <t>PROVIDER_ID</t>
   </si>
@@ -731,6 +731,9 @@
   </si>
   <si>
     <t>xlsx</t>
+  </si>
+  <si>
+    <t>SCHEMA</t>
   </si>
 </sst>
 </file>
@@ -774,11 +777,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1080,10 +1084,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1094,7 +1098,7 @@
     <col min="5" max="5" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1110,8 +1114,11 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1127,8 +1134,11 @@
       <c r="E2" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1144,8 +1154,11 @@
       <c r="E3" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -1161,8 +1174,11 @@
       <c r="E4" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -1178,8 +1194,11 @@
       <c r="E5" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -1195,8 +1214,11 @@
       <c r="E6" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -1212,8 +1234,11 @@
       <c r="E7" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
@@ -1229,8 +1254,11 @@
       <c r="E8" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>33</v>
       </c>
@@ -1246,8 +1274,11 @@
       <c r="E9" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
@@ -1263,8 +1294,11 @@
       <c r="E10" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>41</v>
       </c>
@@ -1280,8 +1314,11 @@
       <c r="E11" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>45</v>
       </c>
@@ -1297,8 +1334,11 @@
       <c r="E12" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>49</v>
       </c>
@@ -1314,8 +1354,11 @@
       <c r="E13" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>53</v>
       </c>
@@ -1331,8 +1374,11 @@
       <c r="E14" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>57</v>
       </c>
@@ -1348,8 +1394,11 @@
       <c r="E15" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>61</v>
       </c>
@@ -1365,8 +1414,11 @@
       <c r="E16" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>65</v>
       </c>
@@ -1382,8 +1434,11 @@
       <c r="E17" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>69</v>
       </c>
@@ -1399,8 +1454,11 @@
       <c r="E18" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>73</v>
       </c>
@@ -1416,8 +1474,11 @@
       <c r="E19" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>77</v>
       </c>
@@ -1433,8 +1494,11 @@
       <c r="E20" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>81</v>
       </c>
@@ -1450,8 +1514,11 @@
       <c r="E21" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>85</v>
       </c>
@@ -1467,8 +1534,11 @@
       <c r="E22" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>89</v>
       </c>
@@ -1484,8 +1554,11 @@
       <c r="E23" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>93</v>
       </c>
@@ -1501,8 +1574,11 @@
       <c r="E24" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>97</v>
       </c>
@@ -1518,8 +1594,11 @@
       <c r="E25" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>101</v>
       </c>
@@ -1535,8 +1614,11 @@
       <c r="E26" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>105</v>
       </c>
@@ -1552,8 +1634,11 @@
       <c r="E27" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>109</v>
       </c>
@@ -1569,8 +1654,11 @@
       <c r="E28" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>113</v>
       </c>
@@ -1586,8 +1674,11 @@
       <c r="E29" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>117</v>
       </c>
@@ -1603,8 +1694,11 @@
       <c r="E30" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>121</v>
       </c>
@@ -1620,8 +1714,11 @@
       <c r="E31" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>125</v>
       </c>
@@ -1637,8 +1734,11 @@
       <c r="E32" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>129</v>
       </c>
@@ -1654,8 +1754,11 @@
       <c r="E33" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>133</v>
       </c>
@@ -1671,8 +1774,11 @@
       <c r="E34" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>137</v>
       </c>
@@ -1688,8 +1794,11 @@
       <c r="E35" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>141</v>
       </c>
@@ -1705,8 +1814,11 @@
       <c r="E36" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>145</v>
       </c>
@@ -1722,8 +1834,11 @@
       <c r="E37" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>149</v>
       </c>
@@ -1739,8 +1854,11 @@
       <c r="E38" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>153</v>
       </c>
@@ -1756,8 +1874,11 @@
       <c r="E39" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>157</v>
       </c>
@@ -1773,8 +1894,11 @@
       <c r="E40" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>161</v>
       </c>
@@ -1790,8 +1914,11 @@
       <c r="E41" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>165</v>
       </c>
@@ -1807,8 +1934,11 @@
       <c r="E42" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>169</v>
       </c>
@@ -1824,8 +1954,11 @@
       <c r="E43" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>173</v>
       </c>
@@ -1841,8 +1974,11 @@
       <c r="E44" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>177</v>
       </c>
@@ -1858,8 +1994,11 @@
       <c r="E45" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>181</v>
       </c>
@@ -1875,8 +2014,11 @@
       <c r="E46" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>185</v>
       </c>
@@ -1892,8 +2034,11 @@
       <c r="E47" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>189</v>
       </c>
@@ -1909,8 +2054,11 @@
       <c r="E48" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>193</v>
       </c>
@@ -1926,8 +2074,11 @@
       <c r="E49" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>197</v>
       </c>
@@ -1943,8 +2094,11 @@
       <c r="E50" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>201</v>
       </c>
@@ -1960,8 +2114,11 @@
       <c r="E51" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>205</v>
       </c>
@@ -1977,8 +2134,11 @@
       <c r="E52" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>209</v>
       </c>
@@ -1994,8 +2154,11 @@
       <c r="E53" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>213</v>
       </c>
@@ -2011,8 +2174,11 @@
       <c r="E54" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>217</v>
       </c>
@@ -2028,8 +2194,11 @@
       <c r="E55" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>221</v>
       </c>
@@ -2045,8 +2214,11 @@
       <c r="E56" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>225</v>
       </c>
@@ -2062,8 +2234,11 @@
       <c r="E57" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>229</v>
       </c>
@@ -2079,8 +2254,11 @@
       <c r="E58" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>233</v>
       </c>
@@ -2095,6 +2273,9 @@
       </c>
       <c r="E59" s="3" t="s">
         <v>237</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Resolved defect with getting fileNameParts
</commit_message>
<xml_diff>
--- a/working/providers/providers.xlsx
+++ b/working/providers/providers.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="150" yWindow="540" windowWidth="20100" windowHeight="6600"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$A$1:$F$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$59</definedName>
   </definedNames>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="297">
   <si>
     <t>PROVIDER_ID</t>
   </si>
@@ -45,9 +49,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>WIRELESS</t>
   </si>
   <si>
@@ -63,9 +64,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>WIRELESS</t>
   </si>
   <si>
@@ -81,9 +79,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>WIRELESS</t>
   </si>
   <si>
@@ -99,9 +94,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>WIRELESS</t>
   </si>
   <si>
@@ -117,9 +109,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>OS3</t>
   </si>
   <si>
@@ -135,9 +124,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>OS3</t>
   </si>
   <si>
@@ -153,9 +139,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>OS3</t>
   </si>
   <si>
@@ -171,9 +154,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>OS3</t>
   </si>
   <si>
@@ -189,9 +169,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>OS3</t>
   </si>
   <si>
@@ -207,9 +184,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>OS3</t>
   </si>
   <si>
@@ -225,9 +199,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>OS3</t>
   </si>
   <si>
@@ -243,9 +214,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>OS3</t>
   </si>
   <si>
@@ -261,9 +229,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>OS3</t>
   </si>
   <si>
@@ -279,9 +244,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>OS3</t>
   </si>
   <si>
@@ -297,9 +259,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>PM</t>
   </si>
   <si>
@@ -315,9 +274,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>PM</t>
   </si>
   <si>
@@ -333,9 +289,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>PM</t>
   </si>
   <si>
@@ -351,9 +304,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>PM</t>
   </si>
   <si>
@@ -369,9 +319,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>PM</t>
   </si>
   <si>
@@ -387,9 +334,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>PM</t>
   </si>
   <si>
@@ -405,9 +349,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>PM</t>
   </si>
   <si>
@@ -423,9 +364,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>PM</t>
   </si>
   <si>
@@ -441,9 +379,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>PM</t>
   </si>
   <si>
@@ -459,9 +394,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>PM</t>
   </si>
   <si>
@@ -477,9 +409,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>PM</t>
   </si>
   <si>
@@ -495,9 +424,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>PM</t>
   </si>
   <si>
@@ -513,9 +439,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>PM</t>
   </si>
   <si>
@@ -531,9 +454,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>JANSAN</t>
   </si>
   <si>
@@ -549,9 +469,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>JANSAN</t>
   </si>
   <si>
@@ -567,9 +484,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>JANSAN</t>
   </si>
   <si>
@@ -585,9 +499,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>JANSAN</t>
   </si>
   <si>
@@ -603,9 +514,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>JANSAN</t>
   </si>
   <si>
@@ -621,9 +529,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>JANSAN</t>
   </si>
   <si>
@@ -639,9 +544,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>JANSAN</t>
   </si>
   <si>
@@ -657,9 +559,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>JANSAN</t>
   </si>
   <si>
@@ -675,9 +574,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>JANSAN</t>
   </si>
   <si>
@@ -693,9 +589,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>JANSAN</t>
   </si>
   <si>
@@ -711,9 +604,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>JANSAN</t>
   </si>
   <si>
@@ -729,9 +619,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>JANSAN</t>
   </si>
   <si>
@@ -747,9 +634,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>JANSAN</t>
   </si>
   <si>
@@ -765,9 +649,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>JANSAN</t>
   </si>
   <si>
@@ -783,9 +664,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>JANSAN</t>
   </si>
   <si>
@@ -801,9 +679,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>JANSAN</t>
   </si>
   <si>
@@ -819,9 +694,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>JANSAN</t>
   </si>
   <si>
@@ -837,9 +709,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>JANSAN</t>
   </si>
   <si>
@@ -855,9 +724,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>MRO</t>
   </si>
   <si>
@@ -873,9 +739,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>MRO</t>
   </si>
   <si>
@@ -891,9 +754,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>MRO</t>
   </si>
   <si>
@@ -909,9 +769,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>MRO</t>
   </si>
   <si>
@@ -927,9 +784,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>MRO</t>
   </si>
   <si>
@@ -945,9 +799,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>MRO</t>
   </si>
   <si>
@@ -963,9 +814,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>MRO</t>
   </si>
   <si>
@@ -981,9 +829,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>MRO</t>
   </si>
   <si>
@@ -999,9 +844,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>MRO</t>
   </si>
   <si>
@@ -1017,9 +859,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>MRO</t>
   </si>
   <si>
@@ -1035,9 +874,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>MRO</t>
   </si>
   <si>
@@ -1053,9 +889,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>DDS3</t>
   </si>
   <si>
@@ -1071,29 +904,32 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>DDS3</t>
+  </si>
+  <si>
+    <t>xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
@@ -1109,1225 +945,1514 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
-    <xf fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1"/>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
-      <alignment/>
-    </xf>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" customWidth="1" max="2" width="22.29"/>
-    <col min="3" customWidth="1" max="3" width="26.43"/>
-    <col min="4" customWidth="1" max="4" width="26.29"/>
-    <col min="5" customWidth="1" max="6" width="23.0"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="6" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c t="s" s="1" r="A1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c t="s" s="1" r="B1">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c t="s" s="1" r="C1">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="2" r="D1">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c t="s" s="2" r="E1">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c t="s" s="2" r="F1">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2">
-      <c t="s" s="2" r="A2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c t="s" s="1" r="B2">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="1" r="C2">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c t="s" s="2" r="D2">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c t="s" s="2" r="E2">
+      <c r="E2" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c t="s" s="1" r="F2">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3">
-      <c t="s" s="2" r="A3">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c t="s" s="1" r="B3">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c t="s" s="1" r="C3">
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c t="s" s="2" r="D3">
+      <c r="E3" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
-      <c t="s" s="2" r="E3">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
-      <c t="s" s="1" r="F3">
+      <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4">
-      <c t="s" s="2" r="A4">
+      <c r="C4" s="1" t="s">
         <v>18</v>
       </c>
-      <c t="s" s="1" r="B4">
+      <c r="D4" s="2" t="s">
         <v>19</v>
       </c>
-      <c t="s" s="1" r="C4">
+      <c r="E4" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>20</v>
       </c>
-      <c t="s" s="2" r="D4">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
-      <c t="s" s="2" r="E4">
+      <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
-      <c t="s" s="1" r="F4">
+      <c r="C5" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5">
-      <c t="s" s="2" r="A5">
+      <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
-      <c t="s" s="1" r="B5">
+      <c r="E5" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>25</v>
       </c>
-      <c t="s" s="1" r="C5">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
-      <c t="s" s="2" r="D5">
+      <c r="B6" s="1" t="s">
         <v>27</v>
       </c>
-      <c t="s" s="2" r="E5">
+      <c r="C6" s="1" t="s">
         <v>28</v>
       </c>
-      <c t="s" s="1" r="F5">
+      <c r="D6" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6">
-      <c t="s" s="2" r="A6">
+      <c r="E6" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>30</v>
       </c>
-      <c t="s" s="1" r="B6">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
-      <c t="s" s="1" r="C6">
+      <c r="B7" s="1" t="s">
         <v>32</v>
       </c>
-      <c t="s" s="2" r="D6">
+      <c r="C7" s="1" t="s">
         <v>33</v>
       </c>
-      <c t="s" s="2" r="E6">
+      <c r="D7" s="2" t="s">
         <v>34</v>
       </c>
-      <c t="s" s="1" r="F6">
+      <c r="E7" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7">
-      <c t="s" s="2" r="A7">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="1" r="B7">
+      <c r="B8" s="1" t="s">
         <v>37</v>
       </c>
-      <c t="s" s="1" r="C7">
+      <c r="C8" s="1" t="s">
         <v>38</v>
       </c>
-      <c t="s" s="2" r="D7">
+      <c r="D8" s="2" t="s">
         <v>39</v>
       </c>
-      <c t="s" s="2" r="E7">
+      <c r="E8" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>40</v>
       </c>
-      <c t="s" s="1" r="F7">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="8">
-      <c t="s" s="2" r="A8">
+      <c r="B9" s="1" t="s">
         <v>42</v>
       </c>
-      <c t="s" s="1" r="B8">
+      <c r="C9" s="1" t="s">
         <v>43</v>
       </c>
-      <c t="s" s="1" r="C8">
+      <c r="D9" s="2" t="s">
         <v>44</v>
       </c>
-      <c t="s" s="2" r="D8">
+      <c r="E9" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>45</v>
       </c>
-      <c t="s" s="2" r="E8">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>46</v>
       </c>
-      <c t="s" s="1" r="F8">
+      <c r="B10" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="9">
-      <c t="s" s="2" r="A9">
+      <c r="C10" s="1" t="s">
         <v>48</v>
       </c>
-      <c t="s" s="1" r="B9">
+      <c r="D10" s="2" t="s">
         <v>49</v>
       </c>
-      <c t="s" s="1" r="C9">
+      <c r="E10" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>50</v>
       </c>
-      <c t="s" s="2" r="D9">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
-      <c t="s" s="2" r="E9">
+      <c r="B11" s="1" t="s">
         <v>52</v>
       </c>
-      <c t="s" s="1" r="F9">
+      <c r="C11" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="10">
-      <c t="s" s="2" r="A10">
+      <c r="D11" s="2" t="s">
         <v>54</v>
       </c>
-      <c t="s" s="1" r="B10">
+      <c r="E11" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>55</v>
       </c>
-      <c t="s" s="1" r="C10">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>56</v>
       </c>
-      <c t="s" s="2" r="D10">
+      <c r="B12" s="1" t="s">
         <v>57</v>
       </c>
-      <c t="s" s="2" r="E10">
+      <c r="C12" s="1" t="s">
         <v>58</v>
       </c>
-      <c t="s" s="1" r="F10">
+      <c r="D12" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="11">
-      <c t="s" s="2" r="A11">
+      <c r="E12" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>60</v>
       </c>
-      <c t="s" s="1" r="B11">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>61</v>
       </c>
-      <c t="s" s="1" r="C11">
+      <c r="B13" s="1" t="s">
         <v>62</v>
       </c>
-      <c t="s" s="2" r="D11">
+      <c r="C13" s="1" t="s">
         <v>63</v>
       </c>
-      <c t="s" s="2" r="E11">
+      <c r="D13" s="2" t="s">
         <v>64</v>
       </c>
-      <c t="s" s="1" r="F11">
+      <c r="E13" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="12">
-      <c t="s" s="2" r="A12">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>66</v>
       </c>
-      <c t="s" s="1" r="B12">
+      <c r="B14" s="1" t="s">
         <v>67</v>
       </c>
-      <c t="s" s="1" r="C12">
+      <c r="C14" s="1" t="s">
         <v>68</v>
       </c>
-      <c t="s" s="2" r="D12">
+      <c r="D14" s="2" t="s">
         <v>69</v>
       </c>
-      <c t="s" s="2" r="E12">
+      <c r="E14" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>70</v>
       </c>
-      <c t="s" s="1" r="F12">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="13">
-      <c t="s" s="2" r="A13">
+      <c r="B15" s="1" t="s">
         <v>72</v>
       </c>
-      <c t="s" s="1" r="B13">
+      <c r="C15" s="1" t="s">
         <v>73</v>
       </c>
-      <c t="s" s="1" r="C13">
+      <c r="D15" s="2" t="s">
         <v>74</v>
       </c>
-      <c t="s" s="2" r="D13">
+      <c r="E15" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>75</v>
       </c>
-      <c t="s" s="2" r="E13">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>76</v>
       </c>
-      <c t="s" s="1" r="F13">
+      <c r="B16" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="14">
-      <c t="s" s="2" r="A14">
+      <c r="C16" s="2" t="s">
         <v>78</v>
       </c>
-      <c t="s" s="1" r="B14">
+      <c r="D16" s="2" t="s">
         <v>79</v>
       </c>
-      <c t="s" s="1" r="C14">
+      <c r="E16" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>80</v>
       </c>
-      <c t="s" s="2" r="D14">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>81</v>
       </c>
-      <c t="s" s="2" r="E14">
+      <c r="B17" s="1" t="s">
         <v>82</v>
       </c>
-      <c t="s" s="1" r="F14">
+      <c r="C17" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="15">
-      <c t="s" s="2" r="A15">
+      <c r="D17" s="2" t="s">
         <v>84</v>
       </c>
-      <c t="s" s="1" r="B15">
+      <c r="E17" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>85</v>
       </c>
-      <c t="s" s="1" r="C15">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>86</v>
       </c>
-      <c t="s" s="2" r="D15">
+      <c r="B18" s="1" t="s">
         <v>87</v>
       </c>
-      <c t="s" s="2" r="E15">
+      <c r="C18" s="2" t="s">
         <v>88</v>
       </c>
-      <c t="s" s="1" r="F15">
+      <c r="D18" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="16">
-      <c t="s" s="2" r="A16">
+      <c r="E18" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>90</v>
       </c>
-      <c t="s" s="1" r="B16">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>91</v>
       </c>
-      <c t="s" s="2" r="C16">
+      <c r="B19" s="1" t="s">
         <v>92</v>
       </c>
-      <c t="s" s="2" r="D16">
+      <c r="C19" s="2" t="s">
         <v>93</v>
       </c>
-      <c t="s" s="2" r="E16">
+      <c r="D19" s="2" t="s">
         <v>94</v>
       </c>
-      <c t="s" s="1" r="F16">
+      <c r="E19" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="17">
-      <c t="s" s="2" r="A17">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>96</v>
       </c>
-      <c t="s" s="1" r="B17">
+      <c r="B20" s="1" t="s">
         <v>97</v>
       </c>
-      <c t="s" s="2" r="C17">
+      <c r="C20" s="2" t="s">
         <v>98</v>
       </c>
-      <c t="s" s="2" r="D17">
+      <c r="D20" s="2" t="s">
         <v>99</v>
       </c>
-      <c t="s" s="2" r="E17">
+      <c r="E20" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>100</v>
       </c>
-      <c t="s" s="1" r="F17">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="18">
-      <c t="s" s="2" r="A18">
+      <c r="B21" s="1" t="s">
         <v>102</v>
       </c>
-      <c t="s" s="1" r="B18">
+      <c r="C21" s="2" t="s">
         <v>103</v>
       </c>
-      <c t="s" s="2" r="C18">
+      <c r="D21" s="2" t="s">
         <v>104</v>
       </c>
-      <c t="s" s="2" r="D18">
+      <c r="E21" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>105</v>
       </c>
-      <c t="s" s="2" r="E18">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>106</v>
       </c>
-      <c t="s" s="1" r="F18">
+      <c r="B22" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="19">
-      <c t="s" s="2" r="A19">
+      <c r="C22" s="2" t="s">
         <v>108</v>
       </c>
-      <c t="s" s="1" r="B19">
+      <c r="D22" s="2" t="s">
         <v>109</v>
       </c>
-      <c t="s" s="2" r="C19">
+      <c r="E22" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>110</v>
       </c>
-      <c t="s" s="2" r="D19">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>111</v>
       </c>
-      <c t="s" s="2" r="E19">
+      <c r="B23" s="1" t="s">
         <v>112</v>
       </c>
-      <c t="s" s="1" r="F19">
+      <c r="C23" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="20">
-      <c t="s" s="2" r="A20">
+      <c r="D23" s="2" t="s">
         <v>114</v>
       </c>
-      <c t="s" s="1" r="B20">
+      <c r="E23" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>115</v>
       </c>
-      <c t="s" s="2" r="C20">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>116</v>
       </c>
-      <c t="s" s="2" r="D20">
+      <c r="B24" s="1" t="s">
         <v>117</v>
       </c>
-      <c t="s" s="2" r="E20">
+      <c r="C24" s="2" t="s">
         <v>118</v>
       </c>
-      <c t="s" s="1" r="F20">
+      <c r="D24" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="21">
-      <c t="s" s="2" r="A21">
+      <c r="E24" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>120</v>
       </c>
-      <c t="s" s="1" r="B21">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>121</v>
       </c>
-      <c t="s" s="2" r="C21">
+      <c r="B25" s="1" t="s">
         <v>122</v>
       </c>
-      <c t="s" s="2" r="D21">
+      <c r="C25" s="2" t="s">
         <v>123</v>
       </c>
-      <c t="s" s="2" r="E21">
+      <c r="D25" s="2" t="s">
         <v>124</v>
       </c>
-      <c t="s" s="1" r="F21">
+      <c r="E25" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="22">
-      <c t="s" s="2" r="A22">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>126</v>
       </c>
-      <c t="s" s="1" r="B22">
+      <c r="B26" s="1" t="s">
         <v>127</v>
       </c>
-      <c t="s" s="2" r="C22">
+      <c r="C26" s="2" t="s">
         <v>128</v>
       </c>
-      <c t="s" s="2" r="D22">
+      <c r="D26" s="2" t="s">
         <v>129</v>
       </c>
-      <c t="s" s="2" r="E22">
+      <c r="E26" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>130</v>
       </c>
-      <c t="s" s="1" r="F22">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="23">
-      <c t="s" s="2" r="A23">
+      <c r="B27" s="1" t="s">
         <v>132</v>
       </c>
-      <c t="s" s="1" r="B23">
+      <c r="C27" s="2" t="s">
         <v>133</v>
       </c>
-      <c t="s" s="2" r="C23">
+      <c r="D27" s="2" t="s">
         <v>134</v>
       </c>
-      <c t="s" s="2" r="D23">
+      <c r="E27" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>135</v>
       </c>
-      <c t="s" s="2" r="E23">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>136</v>
       </c>
-      <c t="s" s="1" r="F23">
+      <c r="B28" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="24">
-      <c t="s" s="2" r="A24">
+      <c r="C28" s="2" t="s">
         <v>138</v>
       </c>
-      <c t="s" s="1" r="B24">
+      <c r="D28" s="2" t="s">
         <v>139</v>
       </c>
-      <c t="s" s="2" r="C24">
+      <c r="E28" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>140</v>
       </c>
-      <c t="s" s="2" r="D24">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>141</v>
       </c>
-      <c t="s" s="2" r="E24">
+      <c r="B29" s="1" t="s">
         <v>142</v>
       </c>
-      <c t="s" s="1" r="F24">
+      <c r="C29" s="2" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="25">
-      <c t="s" s="2" r="A25">
+      <c r="D29" s="2" t="s">
         <v>144</v>
       </c>
-      <c t="s" s="1" r="B25">
+      <c r="E29" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>145</v>
       </c>
-      <c t="s" s="2" r="C25">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>146</v>
       </c>
-      <c t="s" s="2" r="D25">
+      <c r="B30" s="1" t="s">
         <v>147</v>
       </c>
-      <c t="s" s="2" r="E25">
+      <c r="C30" s="2" t="s">
         <v>148</v>
       </c>
-      <c t="s" s="1" r="F25">
+      <c r="D30" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="26">
-      <c t="s" s="2" r="A26">
+      <c r="E30" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>150</v>
       </c>
-      <c t="s" s="1" r="B26">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>151</v>
       </c>
-      <c t="s" s="2" r="C26">
+      <c r="B31" s="1" t="s">
         <v>152</v>
       </c>
-      <c t="s" s="2" r="D26">
+      <c r="C31" s="2" t="s">
         <v>153</v>
       </c>
-      <c t="s" s="2" r="E26">
+      <c r="D31" s="2" t="s">
         <v>154</v>
       </c>
-      <c t="s" s="1" r="F26">
+      <c r="E31" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="27">
-      <c t="s" s="2" r="A27">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>156</v>
       </c>
-      <c t="s" s="1" r="B27">
+      <c r="B32" s="1" t="s">
         <v>157</v>
       </c>
-      <c t="s" s="2" r="C27">
+      <c r="C32" s="2" t="s">
         <v>158</v>
       </c>
-      <c t="s" s="2" r="D27">
+      <c r="D32" s="2" t="s">
         <v>159</v>
       </c>
-      <c t="s" s="2" r="E27">
+      <c r="E32" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>160</v>
       </c>
-      <c t="s" s="1" r="F27">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="28">
-      <c t="s" s="2" r="A28">
+      <c r="B33" s="1" t="s">
         <v>162</v>
       </c>
-      <c t="s" s="1" r="B28">
+      <c r="C33" s="2" t="s">
         <v>163</v>
       </c>
-      <c t="s" s="2" r="C28">
+      <c r="D33" s="2" t="s">
         <v>164</v>
       </c>
-      <c t="s" s="2" r="D28">
+      <c r="E33" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>165</v>
       </c>
-      <c t="s" s="2" r="E28">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
         <v>166</v>
       </c>
-      <c t="s" s="1" r="F28">
+      <c r="B34" s="1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="29">
-      <c t="s" s="2" r="A29">
+      <c r="C34" s="2" t="s">
         <v>168</v>
       </c>
-      <c t="s" s="1" r="B29">
+      <c r="D34" s="2" t="s">
         <v>169</v>
       </c>
-      <c t="s" s="2" r="C29">
+      <c r="E34" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>170</v>
       </c>
-      <c t="s" s="2" r="D29">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>171</v>
       </c>
-      <c t="s" s="2" r="E29">
+      <c r="B35" s="1" t="s">
         <v>172</v>
       </c>
-      <c t="s" s="1" r="F29">
+      <c r="C35" s="2" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="30">
-      <c t="s" s="2" r="A30">
+      <c r="D35" s="2" t="s">
         <v>174</v>
       </c>
-      <c t="s" s="1" r="B30">
+      <c r="E35" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>175</v>
       </c>
-      <c t="s" s="2" r="C30">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>176</v>
       </c>
-      <c t="s" s="2" r="D30">
+      <c r="B36" s="1" t="s">
         <v>177</v>
       </c>
-      <c t="s" s="2" r="E30">
+      <c r="C36" s="2" t="s">
         <v>178</v>
       </c>
-      <c t="s" s="1" r="F30">
+      <c r="D36" s="2" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="31">
-      <c t="s" s="2" r="A31">
+      <c r="E36" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>180</v>
       </c>
-      <c t="s" s="1" r="B31">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>181</v>
       </c>
-      <c t="s" s="2" r="C31">
+      <c r="B37" s="1" t="s">
         <v>182</v>
       </c>
-      <c t="s" s="2" r="D31">
+      <c r="C37" s="2" t="s">
         <v>183</v>
       </c>
-      <c t="s" s="2" r="E31">
+      <c r="D37" s="2" t="s">
         <v>184</v>
       </c>
-      <c t="s" s="1" r="F31">
+      <c r="E37" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="32">
-      <c t="s" s="2" r="A32">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>186</v>
       </c>
-      <c t="s" s="1" r="B32">
+      <c r="B38" s="1" t="s">
         <v>187</v>
       </c>
-      <c t="s" s="2" r="C32">
+      <c r="C38" s="2" t="s">
         <v>188</v>
       </c>
-      <c t="s" s="2" r="D32">
+      <c r="D38" s="2" t="s">
         <v>189</v>
       </c>
-      <c t="s" s="2" r="E32">
+      <c r="E38" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>190</v>
       </c>
-      <c t="s" s="1" r="F32">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="33">
-      <c t="s" s="2" r="A33">
+      <c r="B39" s="1" t="s">
         <v>192</v>
       </c>
-      <c t="s" s="1" r="B33">
+      <c r="C39" s="2" t="s">
         <v>193</v>
       </c>
-      <c t="s" s="2" r="C33">
+      <c r="D39" s="2" t="s">
         <v>194</v>
       </c>
-      <c t="s" s="2" r="D33">
+      <c r="E39" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>195</v>
       </c>
-      <c t="s" s="2" r="E33">
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>196</v>
       </c>
-      <c t="s" s="1" r="F33">
+      <c r="B40" s="1" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="34">
-      <c t="s" s="2" r="A34">
+      <c r="C40" s="2" t="s">
         <v>198</v>
       </c>
-      <c t="s" s="1" r="B34">
+      <c r="D40" s="2" t="s">
         <v>199</v>
       </c>
-      <c t="s" s="2" r="C34">
+      <c r="E40" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>200</v>
       </c>
-      <c t="s" s="2" r="D34">
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
         <v>201</v>
       </c>
-      <c t="s" s="2" r="E34">
+      <c r="B41" s="1" t="s">
         <v>202</v>
       </c>
-      <c t="s" s="1" r="F34">
+      <c r="C41" s="2" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="35">
-      <c t="s" s="2" r="A35">
+      <c r="D41" s="2" t="s">
         <v>204</v>
       </c>
-      <c t="s" s="1" r="B35">
+      <c r="E41" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>205</v>
       </c>
-      <c t="s" s="2" r="C35">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
         <v>206</v>
       </c>
-      <c t="s" s="2" r="D35">
+      <c r="B42" s="1" t="s">
         <v>207</v>
       </c>
-      <c t="s" s="2" r="E35">
+      <c r="C42" s="2" t="s">
         <v>208</v>
       </c>
-      <c t="s" s="1" r="F35">
+      <c r="D42" s="2" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="36">
-      <c t="s" s="2" r="A36">
+      <c r="E42" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>210</v>
       </c>
-      <c t="s" s="1" r="B36">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
         <v>211</v>
       </c>
-      <c t="s" s="2" r="C36">
+      <c r="B43" s="1" t="s">
         <v>212</v>
       </c>
-      <c t="s" s="2" r="D36">
+      <c r="C43" s="2" t="s">
         <v>213</v>
       </c>
-      <c t="s" s="2" r="E36">
+      <c r="D43" s="2" t="s">
         <v>214</v>
       </c>
-      <c t="s" s="1" r="F36">
+      <c r="E43" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="37">
-      <c t="s" s="2" r="A37">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
         <v>216</v>
       </c>
-      <c t="s" s="1" r="B37">
+      <c r="B44" s="1" t="s">
         <v>217</v>
       </c>
-      <c t="s" s="2" r="C37">
+      <c r="C44" s="2" t="s">
         <v>218</v>
       </c>
-      <c t="s" s="2" r="D37">
+      <c r="D44" s="2" t="s">
         <v>219</v>
       </c>
-      <c t="s" s="2" r="E37">
+      <c r="E44" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>220</v>
       </c>
-      <c t="s" s="1" r="F37">
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="38">
-      <c t="s" s="2" r="A38">
+      <c r="B45" s="1" t="s">
         <v>222</v>
       </c>
-      <c t="s" s="1" r="B38">
+      <c r="C45" s="2" t="s">
         <v>223</v>
       </c>
-      <c t="s" s="2" r="C38">
+      <c r="D45" s="2" t="s">
         <v>224</v>
       </c>
-      <c t="s" s="2" r="D38">
+      <c r="E45" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>225</v>
       </c>
-      <c t="s" s="2" r="E38">
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
         <v>226</v>
       </c>
-      <c t="s" s="1" r="F38">
+      <c r="B46" s="1" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="39">
-      <c t="s" s="2" r="A39">
+      <c r="C46" s="2" t="s">
         <v>228</v>
       </c>
-      <c t="s" s="1" r="B39">
+      <c r="D46" s="2" t="s">
         <v>229</v>
       </c>
-      <c t="s" s="2" r="C39">
+      <c r="E46" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>230</v>
       </c>
-      <c t="s" s="2" r="D39">
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
         <v>231</v>
       </c>
-      <c t="s" s="2" r="E39">
+      <c r="B47" s="1" t="s">
         <v>232</v>
       </c>
-      <c t="s" s="1" r="F39">
+      <c r="C47" s="2" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="40">
-      <c t="s" s="2" r="A40">
+      <c r="D47" s="2" t="s">
         <v>234</v>
       </c>
-      <c t="s" s="1" r="B40">
+      <c r="E47" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>235</v>
       </c>
-      <c t="s" s="2" r="C40">
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>236</v>
       </c>
-      <c t="s" s="2" r="D40">
+      <c r="B48" s="1" t="s">
         <v>237</v>
       </c>
-      <c t="s" s="2" r="E40">
+      <c r="C48" s="2" t="s">
         <v>238</v>
       </c>
-      <c t="s" s="1" r="F40">
+      <c r="D48" s="2" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="41">
-      <c t="s" s="2" r="A41">
+      <c r="E48" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F48" s="1" t="s">
         <v>240</v>
       </c>
-      <c t="s" s="1" r="B41">
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>241</v>
       </c>
-      <c t="s" s="2" r="C41">
+      <c r="B49" s="1" t="s">
         <v>242</v>
       </c>
-      <c t="s" s="2" r="D41">
+      <c r="C49" s="2" t="s">
         <v>243</v>
       </c>
-      <c t="s" s="2" r="E41">
+      <c r="D49" s="2" t="s">
         <v>244</v>
       </c>
-      <c t="s" s="1" r="F41">
+      <c r="E49" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="42">
-      <c t="s" s="2" r="A42">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
         <v>246</v>
       </c>
-      <c t="s" s="1" r="B42">
+      <c r="B50" s="1" t="s">
         <v>247</v>
       </c>
-      <c t="s" s="2" r="C42">
+      <c r="C50" s="2" t="s">
         <v>248</v>
       </c>
-      <c t="s" s="2" r="D42">
+      <c r="D50" s="2" t="s">
         <v>249</v>
       </c>
-      <c t="s" s="2" r="E42">
+      <c r="E50" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F50" s="1" t="s">
         <v>250</v>
       </c>
-      <c t="s" s="1" r="F42">
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="43">
-      <c t="s" s="2" r="A43">
+      <c r="B51" s="1" t="s">
         <v>252</v>
       </c>
-      <c t="s" s="1" r="B43">
+      <c r="C51" s="2" t="s">
         <v>253</v>
       </c>
-      <c t="s" s="2" r="C43">
+      <c r="D51" s="2" t="s">
         <v>254</v>
       </c>
-      <c t="s" s="2" r="D43">
+      <c r="E51" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>255</v>
       </c>
-      <c t="s" s="2" r="E43">
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
         <v>256</v>
       </c>
-      <c t="s" s="1" r="F43">
+      <c r="B52" s="1" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="44">
-      <c t="s" s="2" r="A44">
+      <c r="C52" s="2" t="s">
         <v>258</v>
       </c>
-      <c t="s" s="1" r="B44">
+      <c r="D52" s="2" t="s">
         <v>259</v>
       </c>
-      <c t="s" s="2" r="C44">
+      <c r="E52" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>260</v>
       </c>
-      <c t="s" s="2" r="D44">
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
         <v>261</v>
       </c>
-      <c t="s" s="2" r="E44">
+      <c r="B53" s="1" t="s">
         <v>262</v>
       </c>
-      <c t="s" s="1" r="F44">
+      <c r="C53" s="2" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="45">
-      <c t="s" s="2" r="A45">
+      <c r="D53" s="2" t="s">
         <v>264</v>
       </c>
-      <c t="s" s="1" r="B45">
+      <c r="E53" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>265</v>
       </c>
-      <c t="s" s="2" r="C45">
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
         <v>266</v>
       </c>
-      <c t="s" s="2" r="D45">
+      <c r="B54" s="1" t="s">
         <v>267</v>
       </c>
-      <c t="s" s="2" r="E45">
+      <c r="C54" s="2" t="s">
         <v>268</v>
       </c>
-      <c t="s" s="1" r="F45">
+      <c r="D54" s="2" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="46">
-      <c t="s" s="2" r="A46">
+      <c r="E54" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F54" s="1" t="s">
         <v>270</v>
       </c>
-      <c t="s" s="1" r="B46">
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
         <v>271</v>
       </c>
-      <c t="s" s="2" r="C46">
+      <c r="B55" s="1" t="s">
         <v>272</v>
       </c>
-      <c t="s" s="2" r="D46">
+      <c r="C55" s="2" t="s">
         <v>273</v>
       </c>
-      <c t="s" s="2" r="E46">
+      <c r="D55" s="2" t="s">
         <v>274</v>
       </c>
-      <c t="s" s="1" r="F46">
+      <c r="E55" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="47">
-      <c t="s" s="2" r="A47">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
         <v>276</v>
       </c>
-      <c t="s" s="1" r="B47">
+      <c r="B56" s="1" t="s">
         <v>277</v>
       </c>
-      <c t="s" s="2" r="C47">
+      <c r="C56" s="2" t="s">
         <v>278</v>
       </c>
-      <c t="s" s="2" r="D47">
+      <c r="D56" s="2" t="s">
         <v>279</v>
       </c>
-      <c t="s" s="2" r="E47">
+      <c r="E56" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>280</v>
       </c>
-      <c t="s" s="1" r="F47">
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="48">
-      <c t="s" s="2" r="A48">
+      <c r="B57" s="1" t="s">
         <v>282</v>
       </c>
-      <c t="s" s="1" r="B48">
+      <c r="C57" s="2" t="s">
         <v>283</v>
       </c>
-      <c t="s" s="2" r="C48">
+      <c r="D57" s="2" t="s">
         <v>284</v>
       </c>
-      <c t="s" s="2" r="D48">
+      <c r="E57" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F57" s="1" t="s">
         <v>285</v>
       </c>
-      <c t="s" s="2" r="E48">
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
         <v>286</v>
       </c>
-      <c t="s" s="1" r="F48">
+      <c r="B58" s="1" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="49">
-      <c t="s" s="2" r="A49">
+      <c r="C58" s="2" t="s">
         <v>288</v>
       </c>
-      <c t="s" s="1" r="B49">
+      <c r="D58" s="2" t="s">
         <v>289</v>
       </c>
-      <c t="s" s="2" r="C49">
+      <c r="E58" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>290</v>
       </c>
-      <c t="s" s="2" r="D49">
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
         <v>291</v>
       </c>
-      <c t="s" s="2" r="E49">
+      <c r="B59" s="1" t="s">
         <v>292</v>
       </c>
-      <c t="s" s="1" r="F49">
+      <c r="C59" s="2" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="50">
-      <c t="s" s="2" r="A50">
+      <c r="D59" s="2" t="s">
         <v>294</v>
       </c>
-      <c t="s" s="1" r="B50">
+      <c r="E59" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F59" s="1" t="s">
         <v>295</v>
       </c>
-      <c t="s" s="2" r="C50">
-        <v>296</v>
-      </c>
-      <c t="s" s="2" r="D50">
-        <v>297</v>
-      </c>
-      <c t="s" s="2" r="E50">
-        <v>298</v>
-      </c>
-      <c t="s" s="1" r="F50">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="51">
-      <c t="s" s="2" r="A51">
-        <v>300</v>
-      </c>
-      <c t="s" s="1" r="B51">
-        <v>301</v>
-      </c>
-      <c t="s" s="2" r="C51">
-        <v>302</v>
-      </c>
-      <c t="s" s="2" r="D51">
-        <v>303</v>
-      </c>
-      <c t="s" s="2" r="E51">
-        <v>304</v>
-      </c>
-      <c t="s" s="1" r="F51">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="52">
-      <c t="s" s="2" r="A52">
-        <v>306</v>
-      </c>
-      <c t="s" s="1" r="B52">
-        <v>307</v>
-      </c>
-      <c t="s" s="2" r="C52">
-        <v>308</v>
-      </c>
-      <c t="s" s="2" r="D52">
-        <v>309</v>
-      </c>
-      <c t="s" s="2" r="E52">
-        <v>310</v>
-      </c>
-      <c t="s" s="1" r="F52">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="53">
-      <c t="s" s="2" r="A53">
-        <v>312</v>
-      </c>
-      <c t="s" s="1" r="B53">
-        <v>313</v>
-      </c>
-      <c t="s" s="2" r="C53">
-        <v>314</v>
-      </c>
-      <c t="s" s="2" r="D53">
-        <v>315</v>
-      </c>
-      <c t="s" s="2" r="E53">
-        <v>316</v>
-      </c>
-      <c t="s" s="1" r="F53">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="54">
-      <c t="s" s="2" r="A54">
-        <v>318</v>
-      </c>
-      <c t="s" s="1" r="B54">
-        <v>319</v>
-      </c>
-      <c t="s" s="2" r="C54">
-        <v>320</v>
-      </c>
-      <c t="s" s="2" r="D54">
-        <v>321</v>
-      </c>
-      <c t="s" s="2" r="E54">
-        <v>322</v>
-      </c>
-      <c t="s" s="1" r="F54">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="55">
-      <c t="s" s="2" r="A55">
-        <v>324</v>
-      </c>
-      <c t="s" s="1" r="B55">
-        <v>325</v>
-      </c>
-      <c t="s" s="2" r="C55">
-        <v>326</v>
-      </c>
-      <c t="s" s="2" r="D55">
-        <v>327</v>
-      </c>
-      <c t="s" s="2" r="E55">
-        <v>328</v>
-      </c>
-      <c t="s" s="1" r="F55">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="56">
-      <c t="s" s="2" r="A56">
-        <v>330</v>
-      </c>
-      <c t="s" s="1" r="B56">
-        <v>331</v>
-      </c>
-      <c t="s" s="2" r="C56">
-        <v>332</v>
-      </c>
-      <c t="s" s="2" r="D56">
-        <v>333</v>
-      </c>
-      <c t="s" s="2" r="E56">
-        <v>334</v>
-      </c>
-      <c t="s" s="1" r="F56">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="57">
-      <c t="s" s="2" r="A57">
-        <v>336</v>
-      </c>
-      <c t="s" s="1" r="B57">
-        <v>337</v>
-      </c>
-      <c t="s" s="2" r="C57">
-        <v>338</v>
-      </c>
-      <c t="s" s="2" r="D57">
-        <v>339</v>
-      </c>
-      <c t="s" s="2" r="E57">
-        <v>340</v>
-      </c>
-      <c t="s" s="1" r="F57">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="58">
-      <c t="s" s="2" r="A58">
-        <v>342</v>
-      </c>
-      <c t="s" s="1" r="B58">
-        <v>343</v>
-      </c>
-      <c t="s" s="2" r="C58">
-        <v>344</v>
-      </c>
-      <c t="s" s="2" r="D58">
-        <v>345</v>
-      </c>
-      <c t="s" s="2" r="E58">
-        <v>346</v>
-      </c>
-      <c t="s" s="1" r="F58">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="59">
-      <c t="s" s="2" r="A59">
-        <v>348</v>
-      </c>
-      <c t="s" s="1" r="B59">
-        <v>349</v>
-      </c>
-      <c t="s" s="2" r="C59">
-        <v>350</v>
-      </c>
-      <c t="s" s="2" r="D59">
-        <v>351</v>
-      </c>
-      <c t="s" s="2" r="E59">
-        <v>352</v>
-      </c>
-      <c t="s" s="1" r="F59">
-        <v>353</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$F$59"/>
-  <drawing r:id="rId1"/>
+  <autoFilter ref="A1:F59"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated logic of the organizer to retain the original field name. Still need to fix the exporter to use the pretty field name.
</commit_message>
<xml_diff>
--- a/working/providers/providers.xlsx
+++ b/working/providers/providers.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="150" yWindow="540" windowWidth="20100" windowHeight="6600"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$A$1:$F$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$59</definedName>
   </definedNames>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="354">
   <si>
     <t>PROVIDER_ID</t>
   </si>
@@ -729,9 +733,6 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>JANSAN</t>
   </si>
   <si>
@@ -1075,25 +1076,31 @@
   </si>
   <si>
     <t>DDS3</t>
+  </si>
+  <si>
+    <t>xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
@@ -1109,1225 +1116,1514 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
-    <xf fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1"/>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
-      <alignment/>
-    </xf>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" customWidth="1" max="2" width="22.29"/>
-    <col min="3" customWidth="1" max="3" width="26.43"/>
-    <col min="4" customWidth="1" max="4" width="26.29"/>
-    <col min="5" customWidth="1" max="6" width="23.0"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="6" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c t="s" s="1" r="A1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c t="s" s="1" r="B1">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c t="s" s="1" r="C1">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="2" r="D1">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c t="s" s="2" r="E1">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c t="s" s="2" r="F1">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2">
-      <c t="s" s="2" r="A2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c t="s" s="1" r="B2">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="1" r="C2">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c t="s" s="2" r="D2">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c t="s" s="2" r="E2">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c t="s" s="1" r="F2">
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3">
-      <c t="s" s="2" r="A3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c t="s" s="1" r="B3">
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c t="s" s="1" r="C3">
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c t="s" s="2" r="D3">
+      <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
-      <c t="s" s="2" r="E3">
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c t="s" s="1" r="F3">
+      <c r="F3" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4">
-      <c t="s" s="2" r="A4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
-      <c t="s" s="1" r="B4">
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c t="s" s="1" r="C4">
+      <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
-      <c t="s" s="2" r="D4">
+      <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
-      <c t="s" s="2" r="E4">
+      <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
-      <c t="s" s="1" r="F4">
+      <c r="F4" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5">
-      <c t="s" s="2" r="A5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
-      <c t="s" s="1" r="B5">
+      <c r="B5" s="1" t="s">
         <v>25</v>
       </c>
-      <c t="s" s="1" r="C5">
+      <c r="C5" s="1" t="s">
         <v>26</v>
       </c>
-      <c t="s" s="2" r="D5">
+      <c r="D5" s="2" t="s">
         <v>27</v>
       </c>
-      <c t="s" s="2" r="E5">
+      <c r="E5" s="2" t="s">
         <v>28</v>
       </c>
-      <c t="s" s="1" r="F5">
+      <c r="F5" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6">
-      <c t="s" s="2" r="A6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
-      <c t="s" s="1" r="B6">
+      <c r="B6" s="1" t="s">
         <v>31</v>
       </c>
-      <c t="s" s="1" r="C6">
+      <c r="C6" s="1" t="s">
         <v>32</v>
       </c>
-      <c t="s" s="2" r="D6">
+      <c r="D6" s="2" t="s">
         <v>33</v>
       </c>
-      <c t="s" s="2" r="E6">
+      <c r="E6" s="2" t="s">
         <v>34</v>
       </c>
-      <c t="s" s="1" r="F6">
+      <c r="F6" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7">
-      <c t="s" s="2" r="A7">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="1" r="B7">
+      <c r="B7" s="1" t="s">
         <v>37</v>
       </c>
-      <c t="s" s="1" r="C7">
+      <c r="C7" s="1" t="s">
         <v>38</v>
       </c>
-      <c t="s" s="2" r="D7">
+      <c r="D7" s="2" t="s">
         <v>39</v>
       </c>
-      <c t="s" s="2" r="E7">
+      <c r="E7" s="2" t="s">
         <v>40</v>
       </c>
-      <c t="s" s="1" r="F7">
+      <c r="F7" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8">
-      <c t="s" s="2" r="A8">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>42</v>
       </c>
-      <c t="s" s="1" r="B8">
+      <c r="B8" s="1" t="s">
         <v>43</v>
       </c>
-      <c t="s" s="1" r="C8">
+      <c r="C8" s="1" t="s">
         <v>44</v>
       </c>
-      <c t="s" s="2" r="D8">
+      <c r="D8" s="2" t="s">
         <v>45</v>
       </c>
-      <c t="s" s="2" r="E8">
+      <c r="E8" s="2" t="s">
         <v>46</v>
       </c>
-      <c t="s" s="1" r="F8">
+      <c r="F8" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9">
-      <c t="s" s="2" r="A9">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>48</v>
       </c>
-      <c t="s" s="1" r="B9">
+      <c r="B9" s="1" t="s">
         <v>49</v>
       </c>
-      <c t="s" s="1" r="C9">
+      <c r="C9" s="1" t="s">
         <v>50</v>
       </c>
-      <c t="s" s="2" r="D9">
+      <c r="D9" s="2" t="s">
         <v>51</v>
       </c>
-      <c t="s" s="2" r="E9">
+      <c r="E9" s="2" t="s">
         <v>52</v>
       </c>
-      <c t="s" s="1" r="F9">
+      <c r="F9" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10">
-      <c t="s" s="2" r="A10">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>54</v>
       </c>
-      <c t="s" s="1" r="B10">
+      <c r="B10" s="1" t="s">
         <v>55</v>
       </c>
-      <c t="s" s="1" r="C10">
+      <c r="C10" s="1" t="s">
         <v>56</v>
       </c>
-      <c t="s" s="2" r="D10">
+      <c r="D10" s="2" t="s">
         <v>57</v>
       </c>
-      <c t="s" s="2" r="E10">
+      <c r="E10" s="2" t="s">
         <v>58</v>
       </c>
-      <c t="s" s="1" r="F10">
+      <c r="F10" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11">
-      <c t="s" s="2" r="A11">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>60</v>
       </c>
-      <c t="s" s="1" r="B11">
+      <c r="B11" s="1" t="s">
         <v>61</v>
       </c>
-      <c t="s" s="1" r="C11">
+      <c r="C11" s="1" t="s">
         <v>62</v>
       </c>
-      <c t="s" s="2" r="D11">
+      <c r="D11" s="2" t="s">
         <v>63</v>
       </c>
-      <c t="s" s="2" r="E11">
+      <c r="E11" s="2" t="s">
         <v>64</v>
       </c>
-      <c t="s" s="1" r="F11">
+      <c r="F11" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="12">
-      <c t="s" s="2" r="A12">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>66</v>
       </c>
-      <c t="s" s="1" r="B12">
+      <c r="B12" s="1" t="s">
         <v>67</v>
       </c>
-      <c t="s" s="1" r="C12">
+      <c r="C12" s="1" t="s">
         <v>68</v>
       </c>
-      <c t="s" s="2" r="D12">
+      <c r="D12" s="2" t="s">
         <v>69</v>
       </c>
-      <c t="s" s="2" r="E12">
+      <c r="E12" s="2" t="s">
         <v>70</v>
       </c>
-      <c t="s" s="1" r="F12">
+      <c r="F12" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="13">
-      <c t="s" s="2" r="A13">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>72</v>
       </c>
-      <c t="s" s="1" r="B13">
+      <c r="B13" s="1" t="s">
         <v>73</v>
       </c>
-      <c t="s" s="1" r="C13">
+      <c r="C13" s="1" t="s">
         <v>74</v>
       </c>
-      <c t="s" s="2" r="D13">
+      <c r="D13" s="2" t="s">
         <v>75</v>
       </c>
-      <c t="s" s="2" r="E13">
+      <c r="E13" s="2" t="s">
         <v>76</v>
       </c>
-      <c t="s" s="1" r="F13">
+      <c r="F13" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="14">
-      <c t="s" s="2" r="A14">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>78</v>
       </c>
-      <c t="s" s="1" r="B14">
+      <c r="B14" s="1" t="s">
         <v>79</v>
       </c>
-      <c t="s" s="1" r="C14">
+      <c r="C14" s="1" t="s">
         <v>80</v>
       </c>
-      <c t="s" s="2" r="D14">
+      <c r="D14" s="2" t="s">
         <v>81</v>
       </c>
-      <c t="s" s="2" r="E14">
+      <c r="E14" s="2" t="s">
         <v>82</v>
       </c>
-      <c t="s" s="1" r="F14">
+      <c r="F14" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="15">
-      <c t="s" s="2" r="A15">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>84</v>
       </c>
-      <c t="s" s="1" r="B15">
+      <c r="B15" s="1" t="s">
         <v>85</v>
       </c>
-      <c t="s" s="1" r="C15">
+      <c r="C15" s="1" t="s">
         <v>86</v>
       </c>
-      <c t="s" s="2" r="D15">
+      <c r="D15" s="2" t="s">
         <v>87</v>
       </c>
-      <c t="s" s="2" r="E15">
+      <c r="E15" s="2" t="s">
         <v>88</v>
       </c>
-      <c t="s" s="1" r="F15">
+      <c r="F15" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="16">
-      <c t="s" s="2" r="A16">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>90</v>
       </c>
-      <c t="s" s="1" r="B16">
+      <c r="B16" s="1" t="s">
         <v>91</v>
       </c>
-      <c t="s" s="2" r="C16">
+      <c r="C16" s="2" t="s">
         <v>92</v>
       </c>
-      <c t="s" s="2" r="D16">
+      <c r="D16" s="2" t="s">
         <v>93</v>
       </c>
-      <c t="s" s="2" r="E16">
+      <c r="E16" s="2" t="s">
         <v>94</v>
       </c>
-      <c t="s" s="1" r="F16">
+      <c r="F16" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="17">
-      <c t="s" s="2" r="A17">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>96</v>
       </c>
-      <c t="s" s="1" r="B17">
+      <c r="B17" s="1" t="s">
         <v>97</v>
       </c>
-      <c t="s" s="2" r="C17">
+      <c r="C17" s="2" t="s">
         <v>98</v>
       </c>
-      <c t="s" s="2" r="D17">
+      <c r="D17" s="2" t="s">
         <v>99</v>
       </c>
-      <c t="s" s="2" r="E17">
+      <c r="E17" s="2" t="s">
         <v>100</v>
       </c>
-      <c t="s" s="1" r="F17">
+      <c r="F17" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="18">
-      <c t="s" s="2" r="A18">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>102</v>
       </c>
-      <c t="s" s="1" r="B18">
+      <c r="B18" s="1" t="s">
         <v>103</v>
       </c>
-      <c t="s" s="2" r="C18">
+      <c r="C18" s="2" t="s">
         <v>104</v>
       </c>
-      <c t="s" s="2" r="D18">
+      <c r="D18" s="2" t="s">
         <v>105</v>
       </c>
-      <c t="s" s="2" r="E18">
+      <c r="E18" s="2" t="s">
         <v>106</v>
       </c>
-      <c t="s" s="1" r="F18">
+      <c r="F18" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="19">
-      <c t="s" s="2" r="A19">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>108</v>
       </c>
-      <c t="s" s="1" r="B19">
+      <c r="B19" s="1" t="s">
         <v>109</v>
       </c>
-      <c t="s" s="2" r="C19">
+      <c r="C19" s="2" t="s">
         <v>110</v>
       </c>
-      <c t="s" s="2" r="D19">
+      <c r="D19" s="2" t="s">
         <v>111</v>
       </c>
-      <c t="s" s="2" r="E19">
+      <c r="E19" s="2" t="s">
         <v>112</v>
       </c>
-      <c t="s" s="1" r="F19">
+      <c r="F19" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="20">
-      <c t="s" s="2" r="A20">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>114</v>
       </c>
-      <c t="s" s="1" r="B20">
+      <c r="B20" s="1" t="s">
         <v>115</v>
       </c>
-      <c t="s" s="2" r="C20">
+      <c r="C20" s="2" t="s">
         <v>116</v>
       </c>
-      <c t="s" s="2" r="D20">
+      <c r="D20" s="2" t="s">
         <v>117</v>
       </c>
-      <c t="s" s="2" r="E20">
+      <c r="E20" s="2" t="s">
         <v>118</v>
       </c>
-      <c t="s" s="1" r="F20">
+      <c r="F20" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="21">
-      <c t="s" s="2" r="A21">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>120</v>
       </c>
-      <c t="s" s="1" r="B21">
+      <c r="B21" s="1" t="s">
         <v>121</v>
       </c>
-      <c t="s" s="2" r="C21">
+      <c r="C21" s="2" t="s">
         <v>122</v>
       </c>
-      <c t="s" s="2" r="D21">
+      <c r="D21" s="2" t="s">
         <v>123</v>
       </c>
-      <c t="s" s="2" r="E21">
+      <c r="E21" s="2" t="s">
         <v>124</v>
       </c>
-      <c t="s" s="1" r="F21">
+      <c r="F21" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="22">
-      <c t="s" s="2" r="A22">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>126</v>
       </c>
-      <c t="s" s="1" r="B22">
+      <c r="B22" s="1" t="s">
         <v>127</v>
       </c>
-      <c t="s" s="2" r="C22">
+      <c r="C22" s="2" t="s">
         <v>128</v>
       </c>
-      <c t="s" s="2" r="D22">
+      <c r="D22" s="2" t="s">
         <v>129</v>
       </c>
-      <c t="s" s="2" r="E22">
+      <c r="E22" s="2" t="s">
         <v>130</v>
       </c>
-      <c t="s" s="1" r="F22">
+      <c r="F22" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="23">
-      <c t="s" s="2" r="A23">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>132</v>
       </c>
-      <c t="s" s="1" r="B23">
+      <c r="B23" s="1" t="s">
         <v>133</v>
       </c>
-      <c t="s" s="2" r="C23">
+      <c r="C23" s="2" t="s">
         <v>134</v>
       </c>
-      <c t="s" s="2" r="D23">
+      <c r="D23" s="2" t="s">
         <v>135</v>
       </c>
-      <c t="s" s="2" r="E23">
+      <c r="E23" s="2" t="s">
         <v>136</v>
       </c>
-      <c t="s" s="1" r="F23">
+      <c r="F23" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="24">
-      <c t="s" s="2" r="A24">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>138</v>
       </c>
-      <c t="s" s="1" r="B24">
+      <c r="B24" s="1" t="s">
         <v>139</v>
       </c>
-      <c t="s" s="2" r="C24">
+      <c r="C24" s="2" t="s">
         <v>140</v>
       </c>
-      <c t="s" s="2" r="D24">
+      <c r="D24" s="2" t="s">
         <v>141</v>
       </c>
-      <c t="s" s="2" r="E24">
+      <c r="E24" s="2" t="s">
         <v>142</v>
       </c>
-      <c t="s" s="1" r="F24">
+      <c r="F24" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="25">
-      <c t="s" s="2" r="A25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>144</v>
       </c>
-      <c t="s" s="1" r="B25">
+      <c r="B25" s="1" t="s">
         <v>145</v>
       </c>
-      <c t="s" s="2" r="C25">
+      <c r="C25" s="2" t="s">
         <v>146</v>
       </c>
-      <c t="s" s="2" r="D25">
+      <c r="D25" s="2" t="s">
         <v>147</v>
       </c>
-      <c t="s" s="2" r="E25">
+      <c r="E25" s="2" t="s">
         <v>148</v>
       </c>
-      <c t="s" s="1" r="F25">
+      <c r="F25" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="26">
-      <c t="s" s="2" r="A26">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>150</v>
       </c>
-      <c t="s" s="1" r="B26">
+      <c r="B26" s="1" t="s">
         <v>151</v>
       </c>
-      <c t="s" s="2" r="C26">
+      <c r="C26" s="2" t="s">
         <v>152</v>
       </c>
-      <c t="s" s="2" r="D26">
+      <c r="D26" s="2" t="s">
         <v>153</v>
       </c>
-      <c t="s" s="2" r="E26">
+      <c r="E26" s="2" t="s">
         <v>154</v>
       </c>
-      <c t="s" s="1" r="F26">
+      <c r="F26" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="27">
-      <c t="s" s="2" r="A27">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>156</v>
       </c>
-      <c t="s" s="1" r="B27">
+      <c r="B27" s="1" t="s">
         <v>157</v>
       </c>
-      <c t="s" s="2" r="C27">
+      <c r="C27" s="2" t="s">
         <v>158</v>
       </c>
-      <c t="s" s="2" r="D27">
+      <c r="D27" s="2" t="s">
         <v>159</v>
       </c>
-      <c t="s" s="2" r="E27">
+      <c r="E27" s="2" t="s">
         <v>160</v>
       </c>
-      <c t="s" s="1" r="F27">
+      <c r="F27" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="28">
-      <c t="s" s="2" r="A28">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>162</v>
       </c>
-      <c t="s" s="1" r="B28">
+      <c r="B28" s="1" t="s">
         <v>163</v>
       </c>
-      <c t="s" s="2" r="C28">
+      <c r="C28" s="2" t="s">
         <v>164</v>
       </c>
-      <c t="s" s="2" r="D28">
+      <c r="D28" s="2" t="s">
         <v>165</v>
       </c>
-      <c t="s" s="2" r="E28">
+      <c r="E28" s="2" t="s">
         <v>166</v>
       </c>
-      <c t="s" s="1" r="F28">
+      <c r="F28" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="29">
-      <c t="s" s="2" r="A29">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>168</v>
       </c>
-      <c t="s" s="1" r="B29">
+      <c r="B29" s="1" t="s">
         <v>169</v>
       </c>
-      <c t="s" s="2" r="C29">
+      <c r="C29" s="2" t="s">
         <v>170</v>
       </c>
-      <c t="s" s="2" r="D29">
+      <c r="D29" s="2" t="s">
         <v>171</v>
       </c>
-      <c t="s" s="2" r="E29">
+      <c r="E29" s="2" t="s">
         <v>172</v>
       </c>
-      <c t="s" s="1" r="F29">
+      <c r="F29" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="30">
-      <c t="s" s="2" r="A30">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>174</v>
       </c>
-      <c t="s" s="1" r="B30">
+      <c r="B30" s="1" t="s">
         <v>175</v>
       </c>
-      <c t="s" s="2" r="C30">
+      <c r="C30" s="2" t="s">
         <v>176</v>
       </c>
-      <c t="s" s="2" r="D30">
+      <c r="D30" s="2" t="s">
         <v>177</v>
       </c>
-      <c t="s" s="2" r="E30">
+      <c r="E30" s="2" t="s">
         <v>178</v>
       </c>
-      <c t="s" s="1" r="F30">
+      <c r="F30" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="31">
-      <c t="s" s="2" r="A31">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>180</v>
       </c>
-      <c t="s" s="1" r="B31">
+      <c r="B31" s="1" t="s">
         <v>181</v>
       </c>
-      <c t="s" s="2" r="C31">
+      <c r="C31" s="2" t="s">
         <v>182</v>
       </c>
-      <c t="s" s="2" r="D31">
+      <c r="D31" s="2" t="s">
         <v>183</v>
       </c>
-      <c t="s" s="2" r="E31">
+      <c r="E31" s="2" t="s">
         <v>184</v>
       </c>
-      <c t="s" s="1" r="F31">
+      <c r="F31" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="32">
-      <c t="s" s="2" r="A32">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>186</v>
       </c>
-      <c t="s" s="1" r="B32">
+      <c r="B32" s="1" t="s">
         <v>187</v>
       </c>
-      <c t="s" s="2" r="C32">
+      <c r="C32" s="2" t="s">
         <v>188</v>
       </c>
-      <c t="s" s="2" r="D32">
+      <c r="D32" s="2" t="s">
         <v>189</v>
       </c>
-      <c t="s" s="2" r="E32">
+      <c r="E32" s="2" t="s">
         <v>190</v>
       </c>
-      <c t="s" s="1" r="F32">
+      <c r="F32" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="33">
-      <c t="s" s="2" r="A33">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>192</v>
       </c>
-      <c t="s" s="1" r="B33">
+      <c r="B33" s="1" t="s">
         <v>193</v>
       </c>
-      <c t="s" s="2" r="C33">
+      <c r="C33" s="2" t="s">
         <v>194</v>
       </c>
-      <c t="s" s="2" r="D33">
+      <c r="D33" s="2" t="s">
         <v>195</v>
       </c>
-      <c t="s" s="2" r="E33">
+      <c r="E33" s="2" t="s">
         <v>196</v>
       </c>
-      <c t="s" s="1" r="F33">
+      <c r="F33" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="34">
-      <c t="s" s="2" r="A34">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
         <v>198</v>
       </c>
-      <c t="s" s="1" r="B34">
+      <c r="B34" s="1" t="s">
         <v>199</v>
       </c>
-      <c t="s" s="2" r="C34">
+      <c r="C34" s="2" t="s">
         <v>200</v>
       </c>
-      <c t="s" s="2" r="D34">
+      <c r="D34" s="2" t="s">
         <v>201</v>
       </c>
-      <c t="s" s="2" r="E34">
+      <c r="E34" s="2" t="s">
         <v>202</v>
       </c>
-      <c t="s" s="1" r="F34">
+      <c r="F34" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="35">
-      <c t="s" s="2" r="A35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>204</v>
       </c>
-      <c t="s" s="1" r="B35">
+      <c r="B35" s="1" t="s">
         <v>205</v>
       </c>
-      <c t="s" s="2" r="C35">
+      <c r="C35" s="2" t="s">
         <v>206</v>
       </c>
-      <c t="s" s="2" r="D35">
+      <c r="D35" s="2" t="s">
         <v>207</v>
       </c>
-      <c t="s" s="2" r="E35">
+      <c r="E35" s="2" t="s">
         <v>208</v>
       </c>
-      <c t="s" s="1" r="F35">
+      <c r="F35" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="36">
-      <c t="s" s="2" r="A36">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>210</v>
       </c>
-      <c t="s" s="1" r="B36">
+      <c r="B36" s="1" t="s">
         <v>211</v>
       </c>
-      <c t="s" s="2" r="C36">
+      <c r="C36" s="2" t="s">
         <v>212</v>
       </c>
-      <c t="s" s="2" r="D36">
+      <c r="D36" s="2" t="s">
         <v>213</v>
       </c>
-      <c t="s" s="2" r="E36">
+      <c r="E36" s="2" t="s">
         <v>214</v>
       </c>
-      <c t="s" s="1" r="F36">
+      <c r="F36" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="37">
-      <c t="s" s="2" r="A37">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>216</v>
       </c>
-      <c t="s" s="1" r="B37">
+      <c r="B37" s="1" t="s">
         <v>217</v>
       </c>
-      <c t="s" s="2" r="C37">
+      <c r="C37" s="2" t="s">
         <v>218</v>
       </c>
-      <c t="s" s="2" r="D37">
+      <c r="D37" s="2" t="s">
         <v>219</v>
       </c>
-      <c t="s" s="2" r="E37">
+      <c r="E37" s="2" t="s">
         <v>220</v>
       </c>
-      <c t="s" s="1" r="F37">
+      <c r="F37" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="38">
-      <c t="s" s="2" r="A38">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>222</v>
       </c>
-      <c t="s" s="1" r="B38">
+      <c r="B38" s="1" t="s">
         <v>223</v>
       </c>
-      <c t="s" s="2" r="C38">
+      <c r="C38" s="2" t="s">
         <v>224</v>
       </c>
-      <c t="s" s="2" r="D38">
+      <c r="D38" s="2" t="s">
         <v>225</v>
       </c>
-      <c t="s" s="2" r="E38">
+      <c r="E38" s="2" t="s">
         <v>226</v>
       </c>
-      <c t="s" s="1" r="F38">
+      <c r="F38" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="39">
-      <c t="s" s="2" r="A39">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>228</v>
       </c>
-      <c t="s" s="1" r="B39">
+      <c r="B39" s="1" t="s">
         <v>229</v>
       </c>
-      <c t="s" s="2" r="C39">
+      <c r="C39" s="2" t="s">
         <v>230</v>
       </c>
-      <c t="s" s="2" r="D39">
+      <c r="D39" s="2" t="s">
         <v>231</v>
       </c>
-      <c t="s" s="2" r="E39">
+      <c r="E39" s="2" t="s">
         <v>232</v>
       </c>
-      <c t="s" s="1" r="F39">
+      <c r="F39" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="40">
-      <c t="s" s="2" r="A40">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>234</v>
       </c>
-      <c t="s" s="1" r="B40">
+      <c r="B40" s="1" t="s">
         <v>235</v>
       </c>
-      <c t="s" s="2" r="C40">
+      <c r="C40" s="2" t="s">
         <v>236</v>
       </c>
-      <c t="s" s="2" r="D40">
+      <c r="D40" s="2" t="s">
         <v>237</v>
       </c>
-      <c t="s" s="2" r="E40">
+      <c r="E40" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>238</v>
       </c>
-      <c t="s" s="1" r="F40">
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="41">
-      <c t="s" s="2" r="A41">
+      <c r="B41" s="1" t="s">
         <v>240</v>
       </c>
-      <c t="s" s="1" r="B41">
+      <c r="C41" s="2" t="s">
         <v>241</v>
       </c>
-      <c t="s" s="2" r="C41">
+      <c r="D41" s="2" t="s">
         <v>242</v>
       </c>
-      <c t="s" s="2" r="D41">
+      <c r="E41" s="2" t="s">
         <v>243</v>
       </c>
-      <c t="s" s="2" r="E41">
+      <c r="F41" s="1" t="s">
         <v>244</v>
       </c>
-      <c t="s" s="1" r="F41">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="42">
-      <c t="s" s="2" r="A42">
+      <c r="B42" s="1" t="s">
         <v>246</v>
       </c>
-      <c t="s" s="1" r="B42">
+      <c r="C42" s="2" t="s">
         <v>247</v>
       </c>
-      <c t="s" s="2" r="C42">
+      <c r="D42" s="2" t="s">
         <v>248</v>
       </c>
-      <c t="s" s="2" r="D42">
+      <c r="E42" s="2" t="s">
         <v>249</v>
       </c>
-      <c t="s" s="2" r="E42">
+      <c r="F42" s="1" t="s">
         <v>250</v>
       </c>
-      <c t="s" s="1" r="F42">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="43">
-      <c t="s" s="2" r="A43">
+      <c r="B43" s="1" t="s">
         <v>252</v>
       </c>
-      <c t="s" s="1" r="B43">
+      <c r="C43" s="2" t="s">
         <v>253</v>
       </c>
-      <c t="s" s="2" r="C43">
+      <c r="D43" s="2" t="s">
         <v>254</v>
       </c>
-      <c t="s" s="2" r="D43">
+      <c r="E43" s="2" t="s">
         <v>255</v>
       </c>
-      <c t="s" s="2" r="E43">
+      <c r="F43" s="1" t="s">
         <v>256</v>
       </c>
-      <c t="s" s="1" r="F43">
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="44">
-      <c t="s" s="2" r="A44">
+      <c r="B44" s="1" t="s">
         <v>258</v>
       </c>
-      <c t="s" s="1" r="B44">
+      <c r="C44" s="2" t="s">
         <v>259</v>
       </c>
-      <c t="s" s="2" r="C44">
+      <c r="D44" s="2" t="s">
         <v>260</v>
       </c>
-      <c t="s" s="2" r="D44">
+      <c r="E44" s="2" t="s">
         <v>261</v>
       </c>
-      <c t="s" s="2" r="E44">
+      <c r="F44" s="1" t="s">
         <v>262</v>
       </c>
-      <c t="s" s="1" r="F44">
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="45">
-      <c t="s" s="2" r="A45">
+      <c r="B45" s="1" t="s">
         <v>264</v>
       </c>
-      <c t="s" s="1" r="B45">
+      <c r="C45" s="2" t="s">
         <v>265</v>
       </c>
-      <c t="s" s="2" r="C45">
+      <c r="D45" s="2" t="s">
         <v>266</v>
       </c>
-      <c t="s" s="2" r="D45">
+      <c r="E45" s="2" t="s">
         <v>267</v>
       </c>
-      <c t="s" s="2" r="E45">
+      <c r="F45" s="1" t="s">
         <v>268</v>
       </c>
-      <c t="s" s="1" r="F45">
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="46">
-      <c t="s" s="2" r="A46">
+      <c r="B46" s="1" t="s">
         <v>270</v>
       </c>
-      <c t="s" s="1" r="B46">
+      <c r="C46" s="2" t="s">
         <v>271</v>
       </c>
-      <c t="s" s="2" r="C46">
+      <c r="D46" s="2" t="s">
         <v>272</v>
       </c>
-      <c t="s" s="2" r="D46">
+      <c r="E46" s="2" t="s">
         <v>273</v>
       </c>
-      <c t="s" s="2" r="E46">
+      <c r="F46" s="1" t="s">
         <v>274</v>
       </c>
-      <c t="s" s="1" r="F46">
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="47">
-      <c t="s" s="2" r="A47">
+      <c r="B47" s="1" t="s">
         <v>276</v>
       </c>
-      <c t="s" s="1" r="B47">
+      <c r="C47" s="2" t="s">
         <v>277</v>
       </c>
-      <c t="s" s="2" r="C47">
+      <c r="D47" s="2" t="s">
         <v>278</v>
       </c>
-      <c t="s" s="2" r="D47">
+      <c r="E47" s="2" t="s">
         <v>279</v>
       </c>
-      <c t="s" s="2" r="E47">
+      <c r="F47" s="1" t="s">
         <v>280</v>
       </c>
-      <c t="s" s="1" r="F47">
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="48">
-      <c t="s" s="2" r="A48">
+      <c r="B48" s="1" t="s">
         <v>282</v>
       </c>
-      <c t="s" s="1" r="B48">
+      <c r="C48" s="2" t="s">
         <v>283</v>
       </c>
-      <c t="s" s="2" r="C48">
+      <c r="D48" s="2" t="s">
         <v>284</v>
       </c>
-      <c t="s" s="2" r="D48">
+      <c r="E48" s="2" t="s">
         <v>285</v>
       </c>
-      <c t="s" s="2" r="E48">
+      <c r="F48" s="1" t="s">
         <v>286</v>
       </c>
-      <c t="s" s="1" r="F48">
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="49">
-      <c t="s" s="2" r="A49">
+      <c r="B49" s="1" t="s">
         <v>288</v>
       </c>
-      <c t="s" s="1" r="B49">
+      <c r="C49" s="2" t="s">
         <v>289</v>
       </c>
-      <c t="s" s="2" r="C49">
+      <c r="D49" s="2" t="s">
         <v>290</v>
       </c>
-      <c t="s" s="2" r="D49">
+      <c r="E49" s="2" t="s">
         <v>291</v>
       </c>
-      <c t="s" s="2" r="E49">
+      <c r="F49" s="1" t="s">
         <v>292</v>
       </c>
-      <c t="s" s="1" r="F49">
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="50">
-      <c t="s" s="2" r="A50">
+      <c r="B50" s="1" t="s">
         <v>294</v>
       </c>
-      <c t="s" s="1" r="B50">
+      <c r="C50" s="2" t="s">
         <v>295</v>
       </c>
-      <c t="s" s="2" r="C50">
+      <c r="D50" s="2" t="s">
         <v>296</v>
       </c>
-      <c t="s" s="2" r="D50">
+      <c r="E50" s="2" t="s">
         <v>297</v>
       </c>
-      <c t="s" s="2" r="E50">
+      <c r="F50" s="1" t="s">
         <v>298</v>
       </c>
-      <c t="s" s="1" r="F50">
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="51">
-      <c t="s" s="2" r="A51">
+      <c r="B51" s="1" t="s">
         <v>300</v>
       </c>
-      <c t="s" s="1" r="B51">
+      <c r="C51" s="2" t="s">
         <v>301</v>
       </c>
-      <c t="s" s="2" r="C51">
+      <c r="D51" s="2" t="s">
         <v>302</v>
       </c>
-      <c t="s" s="2" r="D51">
+      <c r="E51" s="2" t="s">
         <v>303</v>
       </c>
-      <c t="s" s="2" r="E51">
+      <c r="F51" s="1" t="s">
         <v>304</v>
       </c>
-      <c t="s" s="1" r="F51">
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="52">
-      <c t="s" s="2" r="A52">
+      <c r="B52" s="1" t="s">
         <v>306</v>
       </c>
-      <c t="s" s="1" r="B52">
+      <c r="C52" s="2" t="s">
         <v>307</v>
       </c>
-      <c t="s" s="2" r="C52">
+      <c r="D52" s="2" t="s">
         <v>308</v>
       </c>
-      <c t="s" s="2" r="D52">
+      <c r="E52" s="2" t="s">
         <v>309</v>
       </c>
-      <c t="s" s="2" r="E52">
+      <c r="F52" s="1" t="s">
         <v>310</v>
       </c>
-      <c t="s" s="1" r="F52">
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="53">
-      <c t="s" s="2" r="A53">
+      <c r="B53" s="1" t="s">
         <v>312</v>
       </c>
-      <c t="s" s="1" r="B53">
+      <c r="C53" s="2" t="s">
         <v>313</v>
       </c>
-      <c t="s" s="2" r="C53">
+      <c r="D53" s="2" t="s">
         <v>314</v>
       </c>
-      <c t="s" s="2" r="D53">
+      <c r="E53" s="2" t="s">
         <v>315</v>
       </c>
-      <c t="s" s="2" r="E53">
+      <c r="F53" s="1" t="s">
         <v>316</v>
       </c>
-      <c t="s" s="1" r="F53">
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="54">
-      <c t="s" s="2" r="A54">
+      <c r="B54" s="1" t="s">
         <v>318</v>
       </c>
-      <c t="s" s="1" r="B54">
+      <c r="C54" s="2" t="s">
         <v>319</v>
       </c>
-      <c t="s" s="2" r="C54">
+      <c r="D54" s="2" t="s">
         <v>320</v>
       </c>
-      <c t="s" s="2" r="D54">
+      <c r="E54" s="2" t="s">
         <v>321</v>
       </c>
-      <c t="s" s="2" r="E54">
+      <c r="F54" s="1" t="s">
         <v>322</v>
       </c>
-      <c t="s" s="1" r="F54">
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="55">
-      <c t="s" s="2" r="A55">
+      <c r="B55" s="1" t="s">
         <v>324</v>
       </c>
-      <c t="s" s="1" r="B55">
+      <c r="C55" s="2" t="s">
         <v>325</v>
       </c>
-      <c t="s" s="2" r="C55">
+      <c r="D55" s="2" t="s">
         <v>326</v>
       </c>
-      <c t="s" s="2" r="D55">
+      <c r="E55" s="2" t="s">
         <v>327</v>
       </c>
-      <c t="s" s="2" r="E55">
+      <c r="F55" s="1" t="s">
         <v>328</v>
       </c>
-      <c t="s" s="1" r="F55">
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="56">
-      <c t="s" s="2" r="A56">
+      <c r="B56" s="1" t="s">
         <v>330</v>
       </c>
-      <c t="s" s="1" r="B56">
+      <c r="C56" s="2" t="s">
         <v>331</v>
       </c>
-      <c t="s" s="2" r="C56">
+      <c r="D56" s="2" t="s">
         <v>332</v>
       </c>
-      <c t="s" s="2" r="D56">
+      <c r="E56" s="2" t="s">
         <v>333</v>
       </c>
-      <c t="s" s="2" r="E56">
+      <c r="F56" s="1" t="s">
         <v>334</v>
       </c>
-      <c t="s" s="1" r="F56">
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="57">
-      <c t="s" s="2" r="A57">
+      <c r="B57" s="1" t="s">
         <v>336</v>
       </c>
-      <c t="s" s="1" r="B57">
+      <c r="C57" s="2" t="s">
         <v>337</v>
       </c>
-      <c t="s" s="2" r="C57">
+      <c r="D57" s="2" t="s">
         <v>338</v>
       </c>
-      <c t="s" s="2" r="D57">
+      <c r="E57" s="2" t="s">
         <v>339</v>
       </c>
-      <c t="s" s="2" r="E57">
+      <c r="F57" s="1" t="s">
         <v>340</v>
       </c>
-      <c t="s" s="1" r="F57">
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="58">
-      <c t="s" s="2" r="A58">
+      <c r="B58" s="1" t="s">
         <v>342</v>
       </c>
-      <c t="s" s="1" r="B58">
+      <c r="C58" s="2" t="s">
         <v>343</v>
       </c>
-      <c t="s" s="2" r="C58">
+      <c r="D58" s="2" t="s">
         <v>344</v>
       </c>
-      <c t="s" s="2" r="D58">
+      <c r="E58" s="2" t="s">
         <v>345</v>
       </c>
-      <c t="s" s="2" r="E58">
+      <c r="F58" s="1" t="s">
         <v>346</v>
       </c>
-      <c t="s" s="1" r="F58">
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="59">
-      <c t="s" s="2" r="A59">
+      <c r="B59" s="1" t="s">
         <v>348</v>
       </c>
-      <c t="s" s="1" r="B59">
+      <c r="C59" s="2" t="s">
         <v>349</v>
       </c>
-      <c t="s" s="2" r="C59">
+      <c r="D59" s="2" t="s">
         <v>350</v>
       </c>
-      <c t="s" s="2" r="D59">
+      <c r="E59" s="2" t="s">
         <v>351</v>
       </c>
-      <c t="s" s="2" r="E59">
+      <c r="F59" s="1" t="s">
         <v>352</v>
       </c>
-      <c t="s" s="1" r="F59">
-        <v>353</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$F$59"/>
-  <drawing r:id="rId1"/>
+  <autoFilter ref="A1:F59"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>